<commit_message>
No. of Hit & Misses. Latency yet to be calculated
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-1080" windowWidth="25600" windowHeight="13780" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Q4" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>X - Log of cache size</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>16 * 1024</t>
+  </si>
+  <si>
+    <t>total memory accesses</t>
+  </si>
+  <si>
+    <t>hit</t>
+  </si>
+  <si>
+    <t>miss</t>
   </si>
 </sst>
 </file>
@@ -414,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -425,9 +434,10 @@
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -437,77 +447,143 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>256</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>49642128</v>
+      </c>
+      <c r="E2">
+        <v>35991042</v>
+      </c>
+      <c r="F2">
+        <v>13651086</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>512</v>
       </c>
       <c r="B3">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="E3">
+        <v>38469661</v>
+      </c>
+      <c r="F3">
+        <v>11172467</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1024</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="E4">
+        <v>40482042</v>
+      </c>
+      <c r="F4">
+        <v>9160086</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="E5">
+        <v>45397029</v>
+      </c>
+      <c r="F5">
+        <v>4245099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="E6">
+        <v>46488794</v>
+      </c>
+      <c r="F6">
+        <v>3153334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="E7">
+        <v>47406881</v>
+      </c>
+      <c r="F7">
+        <v>2235247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="E8">
+        <v>48835377</v>
+      </c>
+      <c r="F8">
+        <v>806751</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="E9">
+        <v>49046540</v>
+      </c>
+      <c r="F9">
+        <v>595588</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
         <v>22</v>
+      </c>
+      <c r="E10">
+        <v>49231283</v>
+      </c>
+      <c r="F10">
+        <v>410845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated excel sheet: added graph and part1 and part 2
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>X - Log of cache size</t>
   </si>
@@ -55,16 +55,50 @@
   </si>
   <si>
     <t>miss</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>The cache size should be more than 8Kb for the miss rate to be less than 10%</t>
+  </si>
+  <si>
+    <t>The cache size should be 64Kb or more for the miss rate to be less than 5%</t>
+  </si>
+  <si>
+    <t>Question 4 - Part 1:</t>
+  </si>
+  <si>
+    <t>Question 4 - Part 2:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The miss rate would be reduced by the following ratio: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,18 +121,240 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Y - cache miss rate (%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q4'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q4'!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>27.4989944024962</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.50601948409625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.45224282085571</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.551404162206745</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.352133010897518</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.502721962281714</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.625133797648642</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.199763233356959</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.827613594646869</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2125130584"/>
+        <c:axId val="2113966184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2125130584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2113966184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2113966184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2125130584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,22 +679,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="26.5" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
@@ -458,13 +714,18 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>256</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
+      <c r="C2">
+        <f>F2/D2 * 100</f>
+        <v>27.498994402496201</v>
+      </c>
       <c r="D2">
+        <f>SUM(E2:F2)</f>
         <v>49642128</v>
       </c>
       <c r="E2">
@@ -475,12 +736,20 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>512</v>
       </c>
       <c r="B3">
         <v>9</v>
       </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C10" si="0">F3/D3 * 100</f>
+        <v>22.50601948409625</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="1">SUM(E3:F3)</f>
+        <v>49642128</v>
+      </c>
       <c r="E3">
         <v>38469661</v>
       </c>
@@ -489,12 +758,20 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>1024</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>18.452242820855705</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>49642128</v>
+      </c>
       <c r="E4">
         <v>40482042</v>
       </c>
@@ -503,12 +780,20 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5">
         <v>14</v>
       </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>8.5514041622067456</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>49642128</v>
+      </c>
       <c r="E5">
         <v>45397029</v>
       </c>
@@ -517,12 +802,20 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>6.3521330108975178</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>49642128</v>
+      </c>
       <c r="E6">
         <v>46488794</v>
       </c>
@@ -531,12 +824,20 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <v>16</v>
       </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4.5027219622817141</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>49642128</v>
+      </c>
       <c r="E7">
         <v>47406881</v>
       </c>
@@ -545,12 +846,20 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8">
         <v>20</v>
       </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1.6251337976486424</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>49642128</v>
+      </c>
       <c r="E8">
         <v>48835377</v>
       </c>
@@ -559,12 +868,20 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9">
         <v>21</v>
       </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>1.1997632333569586</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>49642128</v>
+      </c>
       <c r="E9">
         <v>49046540</v>
       </c>
@@ -573,12 +890,20 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10">
         <v>22</v>
       </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.82761359464686923</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>49642128</v>
+      </c>
       <c r="E10">
         <v>49231283</v>
       </c>
@@ -586,8 +911,73 @@
         <v>410845</v>
       </c>
     </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22">
+        <f>C6/C7</f>
+        <v>1.4107317893727178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A22:C22"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updates : Q5 Graph, Q5 part 2, not adding subjective answers
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>X - Log of cache size</t>
   </si>
@@ -73,6 +73,36 @@
   </si>
   <si>
     <t xml:space="preserve">The miss rate would be reduced by the following ratio: </t>
+  </si>
+  <si>
+    <t>CPI Latency 10</t>
+  </si>
+  <si>
+    <t>CPI Latency 25</t>
+  </si>
+  <si>
+    <t>CPI Latency 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPI = </t>
+  </si>
+  <si>
+    <t>Q 5:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part 2: </t>
+  </si>
+  <si>
+    <t>Latency 10</t>
+  </si>
+  <si>
+    <t>Latency 25</t>
+  </si>
+  <si>
+    <t>Latency 100</t>
+  </si>
+  <si>
+    <t>Speed up from 32 KB to 64 KB</t>
   </si>
 </sst>
 </file>
@@ -104,12 +134,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,19 +180,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -270,11 +333,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2125130584"/>
-        <c:axId val="2113966184"/>
+        <c:axId val="2100381032"/>
+        <c:axId val="2100391992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2125130584"/>
+        <c:axId val="2100381032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -284,12 +347,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113966184"/>
+        <c:crossAx val="2100391992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2113966184"/>
+        <c:axId val="2100391992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,7 +363,351 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125130584"/>
+        <c:crossAx val="2100381032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPI Latency 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q4'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q4'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.474909496224658</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.025541753568662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.660701853877013</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.769626374598607</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.571691970980777</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.405244976605354</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.146262041788378</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.107978691002126</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.074485223518218</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPI Latency 25</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q4'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q4'!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8.59975865659909</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.4014446761831</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.428538277005369</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.052336998929619</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.524511922615404</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.080653270947612</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.390032111435674</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.28794317600567</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.198627262715249</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q4'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPI Latency 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q4'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q4'!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>29.22400445847124</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.28095928925529</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.26772039264715</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.46589012058468</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.288611680788543</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.457694742658897</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.608882459672156</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.187765601023389</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8193374587004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2109861752"/>
+        <c:axId val="2106232808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2109861752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2106232808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2106232808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2109861752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -326,16 +733,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1435100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -349,6 +756,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -679,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -691,29 +1128,41 @@
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="26.5" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>256</v>
       </c>
@@ -734,8 +1183,20 @@
       <c r="F2">
         <v>13651086</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <f>(G$12+(E2/D2)+(F2/D2)*10)</f>
+        <v>4.4749094962246581</v>
+      </c>
+      <c r="H2">
+        <f>(G$12+(E2/D2)+(F2/D2)*25)</f>
+        <v>8.5997586565990893</v>
+      </c>
+      <c r="I2">
+        <f>(G$12+(E2/D2)+(F2/D2)*100)</f>
+        <v>29.224004458471239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>512</v>
       </c>
@@ -756,8 +1217,20 @@
       <c r="F3">
         <v>11172467</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <f t="shared" ref="G3:G10" si="2">(G$12+(E3/D3)+(F3/D3)*10)</f>
+        <v>4.0255417535686622</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H10" si="3">(G$12+(E3/D3)+(F3/D3)*25)</f>
+        <v>7.4014446761831003</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I10" si="4">(G$12+(E3/D3)+(F3/D3)*100)</f>
+        <v>24.280959289255286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>1024</v>
       </c>
@@ -778,8 +1251,20 @@
       <c r="F4">
         <v>9160086</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>3.6607018538770135</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>6.4285382770053694</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="4"/>
+        <v>20.267720392647149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -800,8 +1285,20 @@
       <c r="F5">
         <v>4245099</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>2.7696263745986069</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>4.0523369989296185</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>10.465890120584678</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -822,8 +1319,20 @@
       <c r="F6">
         <v>3153334</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>2.5716919709807766</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>3.524511922615404</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>8.2886116807885433</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -844,8 +1353,20 @@
       <c r="F7">
         <v>2235247</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>2.4052449766053545</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>3.0806532709476118</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>6.4576947426588971</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -866,8 +1387,20 @@
       <c r="F8">
         <v>806751</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>2.1462620417883778</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>2.3900321114356742</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>3.6088824596721558</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -888,8 +1421,20 @@
       <c r="F9">
         <v>595588</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>2.1079786910021263</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>2.2879431760056699</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>3.187765601023389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -910,63 +1455,118 @@
       <c r="F10">
         <v>410845</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>2.0744852235182183</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>2.1986272627152488</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="4"/>
+        <v>2.8193374587004003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="F12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="4" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="4" t="s">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="5" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="4" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="12">
         <f>C6/C7</f>
         <v>1.4107317893727178</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+    <row r="23" spans="1:10">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="F30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="30">
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H31">
+        <f>(G6/G7)</f>
+        <v>1.0692016804917466</v>
+      </c>
+      <c r="I31">
+        <f>(H6/H7)</f>
+        <v>1.1440793924631645</v>
+      </c>
+      <c r="J31">
+        <f>(I6/I7)</f>
+        <v>1.2835248507543704</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Question 6, along with stats
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Q4" sheetId="1" r:id="rId1"/>
+    <sheet name="Q6" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>X - Log of cache size</t>
   </si>
@@ -103,13 +104,49 @@
   </si>
   <si>
     <t>Speed up from 32 KB to 64 KB</t>
+  </si>
+  <si>
+    <t>Cache Size</t>
+  </si>
+  <si>
+    <t>Num Misses</t>
+  </si>
+  <si>
+    <t>Write Through</t>
+  </si>
+  <si>
+    <t>Num of Store Instructions</t>
+  </si>
+  <si>
+    <t>Total memory operations</t>
+  </si>
+  <si>
+    <t>No. of Dirty Evictions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> into cache(numMiss*64)</t>
+  </si>
+  <si>
+    <t>out of cache(numStores*4)</t>
+  </si>
+  <si>
+    <t>into cache(numMiss*64)</t>
+  </si>
+  <si>
+    <t>out of cache(numDirtyEvictions * 64)</t>
+  </si>
+  <si>
+    <t>Write Back</t>
+  </si>
+  <si>
+    <t>Total Data Traffic/Memory Op</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,8 +170,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +217,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD5B4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -175,12 +233,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -191,21 +279,65 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -333,11 +465,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2100381032"/>
-        <c:axId val="2100391992"/>
+        <c:axId val="-2127067432"/>
+        <c:axId val="-2127064472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2100381032"/>
+        <c:axId val="-2127067432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -347,12 +479,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100391992"/>
+        <c:crossAx val="-2127064472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2100391992"/>
+        <c:axId val="-2127064472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -363,7 +495,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100381032"/>
+        <c:crossAx val="-2127067432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -677,11 +809,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2109861752"/>
-        <c:axId val="2106232808"/>
+        <c:axId val="2130008824"/>
+        <c:axId val="2124104440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2109861752"/>
+        <c:axId val="2130008824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -691,12 +823,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106232808"/>
+        <c:crossAx val="2124104440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2106232808"/>
+        <c:axId val="2124104440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -707,7 +839,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109861752"/>
+        <c:crossAx val="2130008824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1118,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1477,52 +1609,52 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="12">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="10">
         <f>C6/C7</f>
         <v>1.4107317893727178</v>
       </c>
@@ -1584,4 +1716,525 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1"/>
+    <col min="8" max="8" width="23.83203125" customWidth="1"/>
+    <col min="9" max="9" width="27.6640625" customWidth="1"/>
+    <col min="10" max="10" width="23.1640625" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="12" max="12" width="34.6640625" customWidth="1"/>
+    <col min="13" max="13" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="13"/>
+      <c r="I1" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="16"/>
+      <c r="M1" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1">
+        <v>256</v>
+      </c>
+      <c r="B3" s="1">
+        <v>256</v>
+      </c>
+      <c r="C3" s="14">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>13651086</v>
+      </c>
+      <c r="E3" s="14">
+        <v>49642128</v>
+      </c>
+      <c r="F3">
+        <v>21611962</v>
+      </c>
+      <c r="G3">
+        <f>D3*64</f>
+        <v>873669504</v>
+      </c>
+      <c r="H3">
+        <f>F3*4</f>
+        <v>86447848</v>
+      </c>
+      <c r="I3">
+        <f>(G3+H3)/E3</f>
+        <v>19.340777494470018</v>
+      </c>
+      <c r="J3">
+        <v>4676824</v>
+      </c>
+      <c r="K3">
+        <f>D3*64</f>
+        <v>873669504</v>
+      </c>
+      <c r="L3">
+        <f>J3*64</f>
+        <v>299316736</v>
+      </c>
+      <c r="M3">
+        <f>(K3+L3)/E3</f>
+        <v>23.628846853624001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1">
+        <v>512</v>
+      </c>
+      <c r="B4" s="1">
+        <v>512</v>
+      </c>
+      <c r="C4" s="14">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>11172467</v>
+      </c>
+      <c r="E4" s="14">
+        <v>49642128</v>
+      </c>
+      <c r="F4">
+        <v>21611962</v>
+      </c>
+      <c r="G4">
+        <f>D4*64</f>
+        <v>715037888</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H11" si="0">F4*4</f>
+        <v>86447848</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I11" si="1">(G4+H4)/E4</f>
+        <v>16.14527354669405</v>
+      </c>
+      <c r="J4">
+        <v>3789508</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K11" si="2">D4*64</f>
+        <v>715037888</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L11" si="3">J4*64</f>
+        <v>242528512</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M11" si="4">(K4+L4)/E4</f>
+        <v>19.289390656258732</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1024</v>
+      </c>
+      <c r="C5" s="14">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>9160086</v>
+      </c>
+      <c r="E5" s="14">
+        <v>49642128</v>
+      </c>
+      <c r="F5">
+        <v>21611962</v>
+      </c>
+      <c r="G5">
+        <f>D5*64</f>
+        <v>586245504</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>86447848</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>13.550856482220102</v>
+      </c>
+      <c r="J5">
+        <v>3148608</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>586245504</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>201510912</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="4"/>
+        <v>15.868707642831104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <f>16*1024</f>
+        <v>16384</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="14">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>4245099</v>
+      </c>
+      <c r="E6" s="14">
+        <v>49642128</v>
+      </c>
+      <c r="F6">
+        <v>21611962</v>
+      </c>
+      <c r="G6">
+        <f>D6*64</f>
+        <v>271686336</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>86447848</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>7.2143197406847666</v>
+      </c>
+      <c r="J6">
+        <v>1688401</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>271686336</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>108057664</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="4"/>
+        <v>7.6496317804909575</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <f>32*1024</f>
+        <v>32768</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="14">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>3153334</v>
+      </c>
+      <c r="E7" s="14">
+        <v>49642128</v>
+      </c>
+      <c r="F7">
+        <v>21611962</v>
+      </c>
+      <c r="G7">
+        <f>D7*64</f>
+        <v>201813376</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>86447848</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>5.8067862038468618</v>
+      </c>
+      <c r="J7">
+        <v>1241321</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>201813376</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>79444544</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="4"/>
+        <v>5.665710382117382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <f>64*1024</f>
+        <v>65536</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="14">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>2235247</v>
+      </c>
+      <c r="E8" s="14">
+        <v>49642128</v>
+      </c>
+      <c r="F8">
+        <v>21611962</v>
+      </c>
+      <c r="G8">
+        <f>D8*64</f>
+        <v>143055808</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>86447848</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>4.6231631327327465</v>
+      </c>
+      <c r="J8">
+        <v>888405</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>143055808</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>56857920</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="4"/>
+        <v>4.0270982742722072</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <f>1024*1024</f>
+        <v>1048576</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="14">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>806751</v>
+      </c>
+      <c r="E9" s="14">
+        <v>49642128</v>
+      </c>
+      <c r="F9">
+        <v>21611962</v>
+      </c>
+      <c r="G9">
+        <f>D9*64</f>
+        <v>51632064</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>86447848</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>2.7815067073675812</v>
+      </c>
+      <c r="J9">
+        <v>374593</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>51632064</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>23973952</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>1.5230212532387815</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <f>2*1024*1024</f>
+        <v>2097152</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14">
+        <v>21</v>
+      </c>
+      <c r="D10">
+        <v>595588</v>
+      </c>
+      <c r="E10" s="14">
+        <v>49642128</v>
+      </c>
+      <c r="F10">
+        <v>21611962</v>
+      </c>
+      <c r="G10">
+        <f>D10*64</f>
+        <v>38117632</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>86447848</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>2.5092695462209034</v>
+      </c>
+      <c r="J10">
+        <v>323427</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>38117632</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>20699328</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>1.1848194742981204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11">
+        <f>4*1024*1024</f>
+        <v>4194304</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="14">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>410845</v>
+      </c>
+      <c r="E11" s="14">
+        <v>49642128</v>
+      </c>
+      <c r="F11">
+        <v>21611962</v>
+      </c>
+      <c r="G11">
+        <f>D11*64</f>
+        <v>26294080</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>86447848</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>2.2710937774464464</v>
+      </c>
+      <c r="J11">
+        <v>260065</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>26294080</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>16644160</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="4"/>
+        <v>0.86495566829850645</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="C12" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Q7 and Q8 plus some bug fixes
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Q4" sheetId="1" r:id="rId1"/>
     <sheet name="Q6" sheetId="2" r:id="rId2"/>
+    <sheet name="Q8" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
   <si>
     <t>X - Log of cache size</t>
   </si>
@@ -140,6 +141,63 @@
   </si>
   <si>
     <t>Total Data Traffic/Memory Op</t>
+  </si>
+  <si>
+    <t>Hit</t>
+  </si>
+  <si>
+    <t>Miss</t>
+  </si>
+  <si>
+    <t>Block Size</t>
+  </si>
+  <si>
+    <t>8KB</t>
+  </si>
+  <si>
+    <t>32KB</t>
+  </si>
+  <si>
+    <t>Total Accesses</t>
+  </si>
+  <si>
+    <t>Log cache blokc size</t>
+  </si>
+  <si>
+    <t>Miss Rate 8KB</t>
+  </si>
+  <si>
+    <t>Miss Rate 32 KB</t>
+  </si>
+  <si>
+    <t>NumStores</t>
+  </si>
+  <si>
+    <t>NumMisses</t>
+  </si>
+  <si>
+    <t>Dirty Evictions</t>
+  </si>
+  <si>
+    <t>total data traffic/memops write through  8KB</t>
+  </si>
+  <si>
+    <t>total data traffic/memops write back  8KB</t>
+  </si>
+  <si>
+    <t>total data traffic/memops write through  32KB</t>
+  </si>
+  <si>
+    <t>total data traffic/memops write back 32KB</t>
+  </si>
+  <si>
+    <t>Q1: Blck Size is 256B</t>
+  </si>
+  <si>
+    <t>Q2: Block Size is 256B</t>
+  </si>
+  <si>
+    <t>2-way cache</t>
   </si>
 </sst>
 </file>
@@ -233,8 +291,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -284,6 +362,11 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,19 +376,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -322,6 +400,16 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -338,6 +426,16 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -360,7 +458,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -465,11 +562,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127067432"/>
-        <c:axId val="-2127064472"/>
+        <c:axId val="2064810888"/>
+        <c:axId val="2064805144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2127067432"/>
+        <c:axId val="2064810888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -479,12 +576,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127064472"/>
+        <c:crossAx val="2064805144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127064472"/>
+        <c:axId val="2064805144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,14 +592,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127067432"/>
+        <c:crossAx val="2064810888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -809,11 +905,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2130008824"/>
-        <c:axId val="2124104440"/>
+        <c:axId val="2066574520"/>
+        <c:axId val="2066577512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2130008824"/>
+        <c:axId val="2066574520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,12 +919,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124104440"/>
+        <c:crossAx val="2066577512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2124104440"/>
+        <c:axId val="2066577512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,7 +935,774 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130008824"/>
+        <c:crossAx val="2066574520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Miss Rate 8KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8'!$E$2:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>43.41334440779815</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.57276521264358</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.14515219814912</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.961877218478627</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.501823531819586</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.660378942659348</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.491341064186451</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.328285443363749</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.052822715416228</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Miss Rate 32 KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8'!$L$2:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20.01411784764747</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.55695275593343</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.712899737094268</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.203881590249314</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.947047878366536</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.354829108051129</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.150315312832681</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.349249169979176</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.940102164838703</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2066614728"/>
+        <c:axId val="2066617720"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2066614728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2066617720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2066617720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2066614728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8'!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total data traffic/memops write back  8KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8'!$V$2:$V$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>43.36844222310534</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.37769533167474</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.88116673805764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.670745782694892</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.18836904010239</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.303955060105401</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.077631160372496</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.764316308116364</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.167568320197716</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8'!$AE$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total data traffic/memops write back 32KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8'!$AE$2:$AE$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20.17534010629037</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.56267241404317</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.657057086674447</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.125233309901622</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.851899338400642</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.244246419089851</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.02184048193905</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.182335132772713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.663385904810527</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2074806984"/>
+        <c:axId val="2065597112"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2074806984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2065597112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2065597112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2074806984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8'!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total data traffic/memops write through  8KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8'!$T$2:$T$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>29.52596149786327</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.18799081296434</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.514318483687887</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.197022496698771</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.622588137236986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.084063600174432</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.975879357951778</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.511523760625249</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.615227614738836</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8'!$AB$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total data traffic/memops write through  32KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8'!$AB$2:$AB$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>14.55045649936683</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.497870840669843</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.397676908612781</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.791905294632011</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.987531719027032</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.608511706025172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.477622877085366</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.604940545659122</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.98308646236922</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2066300776"/>
+        <c:axId val="2066263944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2066300776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2066263944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2066263944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2066300776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -918,6 +1781,101 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>1828800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1609,12 +2567,12 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="8" t="s">
@@ -1625,20 +2583,20 @@
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="9" t="s">
@@ -1649,11 +2607,11 @@
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="10">
         <f>C6/C7</f>
         <v>1.4107317893727178</v>
@@ -1722,8 +2680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView showRuler="0" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1748,7 +2706,7 @@
       <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
@@ -1760,21 +2718,21 @@
       <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="12" t="s">
         <v>39</v>
       </c>
       <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="16"/>
-      <c r="M1" s="17" t="s">
+      <c r="L1" s="18"/>
+      <c r="M1" s="12" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1799,20 +2757,20 @@
       <c r="B3" s="1">
         <v>256</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="11">
         <v>8</v>
       </c>
       <c r="D3">
         <v>13651086</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="11">
         <v>49642128</v>
       </c>
       <c r="F3">
         <v>21611962</v>
       </c>
       <c r="G3">
-        <f>D3*64</f>
+        <f t="shared" ref="G3:G11" si="0">D3*64</f>
         <v>873669504</v>
       </c>
       <c r="H3">
@@ -1846,43 +2804,43 @@
       <c r="B4" s="1">
         <v>512</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>9</v>
       </c>
       <c r="D4">
         <v>11172467</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="11">
         <v>49642128</v>
       </c>
       <c r="F4">
         <v>21611962</v>
       </c>
       <c r="G4">
-        <f>D4*64</f>
+        <f t="shared" si="0"/>
         <v>715037888</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H11" si="0">F4*4</f>
+        <f t="shared" ref="H4:H11" si="1">F4*4</f>
         <v>86447848</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I11" si="1">(G4+H4)/E4</f>
+        <f t="shared" ref="I4:I11" si="2">(G4+H4)/E4</f>
         <v>16.14527354669405</v>
       </c>
       <c r="J4">
         <v>3789508</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K11" si="2">D4*64</f>
+        <f t="shared" ref="K4:K11" si="3">D4*64</f>
         <v>715037888</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L11" si="3">J4*64</f>
+        <f t="shared" ref="L4:L11" si="4">J4*64</f>
         <v>242528512</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M11" si="4">(K4+L4)/E4</f>
+        <f t="shared" ref="M4:M11" si="5">(K4+L4)/E4</f>
         <v>19.289390656258732</v>
       </c>
     </row>
@@ -1893,43 +2851,43 @@
       <c r="B5" s="1">
         <v>1024</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="11">
         <v>10</v>
       </c>
       <c r="D5">
         <v>9160086</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="11">
         <v>49642128</v>
       </c>
       <c r="F5">
         <v>21611962</v>
       </c>
       <c r="G5">
-        <f>D5*64</f>
+        <f t="shared" si="0"/>
         <v>586245504</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86447848</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.550856482220102</v>
       </c>
       <c r="J5">
         <v>3148608</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>586245504</v>
       </c>
       <c r="L5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>201510912</v>
       </c>
       <c r="M5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>15.868707642831104</v>
       </c>
     </row>
@@ -1941,43 +2899,43 @@
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>14</v>
       </c>
       <c r="D6">
         <v>4245099</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="11">
         <v>49642128</v>
       </c>
       <c r="F6">
         <v>21611962</v>
       </c>
       <c r="G6">
-        <f>D6*64</f>
+        <f t="shared" si="0"/>
         <v>271686336</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86447848</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.2143197406847666</v>
       </c>
       <c r="J6">
         <v>1688401</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>271686336</v>
       </c>
       <c r="L6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>108057664</v>
       </c>
       <c r="M6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.6496317804909575</v>
       </c>
     </row>
@@ -1989,43 +2947,43 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="11">
         <v>15</v>
       </c>
       <c r="D7">
         <v>3153334</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="11">
         <v>49642128</v>
       </c>
       <c r="F7">
         <v>21611962</v>
       </c>
       <c r="G7">
-        <f>D7*64</f>
+        <f t="shared" si="0"/>
         <v>201813376</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86447848</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.8067862038468618</v>
       </c>
       <c r="J7">
         <v>1241321</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>201813376</v>
       </c>
       <c r="L7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>79444544</v>
       </c>
       <c r="M7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.665710382117382</v>
       </c>
     </row>
@@ -2037,43 +2995,43 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="11">
         <v>16</v>
       </c>
       <c r="D8">
         <v>2235247</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="11">
         <v>49642128</v>
       </c>
       <c r="F8">
         <v>21611962</v>
       </c>
       <c r="G8">
-        <f>D8*64</f>
+        <f t="shared" si="0"/>
         <v>143055808</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86447848</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.6231631327327465</v>
       </c>
       <c r="J8">
         <v>888405</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>143055808</v>
       </c>
       <c r="L8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>56857920</v>
       </c>
       <c r="M8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0270982742722072</v>
       </c>
     </row>
@@ -2085,43 +3043,43 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="11">
         <v>20</v>
       </c>
       <c r="D9">
         <v>806751</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="11">
         <v>49642128</v>
       </c>
       <c r="F9">
         <v>21611962</v>
       </c>
       <c r="G9">
-        <f>D9*64</f>
+        <f t="shared" si="0"/>
         <v>51632064</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86447848</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.7815067073675812</v>
       </c>
       <c r="J9">
         <v>374593</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>51632064</v>
       </c>
       <c r="L9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23973952</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5230212532387815</v>
       </c>
     </row>
@@ -2133,43 +3091,43 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="11">
         <v>21</v>
       </c>
       <c r="D10">
         <v>595588</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="11">
         <v>49642128</v>
       </c>
       <c r="F10">
         <v>21611962</v>
       </c>
       <c r="G10">
-        <f>D10*64</f>
+        <f t="shared" si="0"/>
         <v>38117632</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86447848</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5092695462209034</v>
       </c>
       <c r="J10">
         <v>323427</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38117632</v>
       </c>
       <c r="L10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20699328</v>
       </c>
       <c r="M10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1848194742981204</v>
       </c>
     </row>
@@ -2181,43 +3139,43 @@
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="11">
         <v>22</v>
       </c>
       <c r="D11">
         <v>410845</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="11">
         <v>49642128</v>
       </c>
       <c r="F11">
         <v>21611962</v>
       </c>
       <c r="G11">
-        <f>D11*64</f>
+        <f t="shared" si="0"/>
         <v>26294080</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86447848</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.2710937774464464</v>
       </c>
       <c r="J11">
         <v>260065</v>
       </c>
       <c r="K11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26294080</v>
       </c>
       <c r="L11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16644160</v>
       </c>
       <c r="M11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.86495566829850645</v>
       </c>
     </row>
@@ -2237,4 +3195,987 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="12" max="12" width="15.5" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
+    <col min="19" max="19" width="22.6640625" customWidth="1"/>
+    <col min="20" max="20" width="32.6640625" customWidth="1"/>
+    <col min="21" max="21" width="13.83203125" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" customWidth="1"/>
+    <col min="30" max="30" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>28090820</v>
+      </c>
+      <c r="D2">
+        <f>F2-C2</f>
+        <v>21551308</v>
+      </c>
+      <c r="E2">
+        <f>D2/F2*100</f>
+        <v>43.413344407798149</v>
+      </c>
+      <c r="F2">
+        <v>49642128</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>39706694</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K10" si="0">M2-J2</f>
+        <v>9935434</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L10" si="1">K2/M2*100</f>
+        <v>20.014117847647466</v>
+      </c>
+      <c r="M2">
+        <v>49642128</v>
+      </c>
+      <c r="O2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2">
+        <v>4</v>
+      </c>
+      <c r="Q2">
+        <v>21611962</v>
+      </c>
+      <c r="R2">
+        <v>21551308</v>
+      </c>
+      <c r="S2" s="11">
+        <v>49642128</v>
+      </c>
+      <c r="T2">
+        <f>(R2*64 + Q2* 4)/S2</f>
+        <v>29.525961497863268</v>
+      </c>
+      <c r="U2">
+        <v>12087782</v>
+      </c>
+      <c r="V2">
+        <f>(R2*64 + U2 *64)/S2</f>
+        <v>43.36844222310534</v>
+      </c>
+      <c r="X2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y2">
+        <v>4</v>
+      </c>
+      <c r="Z2">
+        <v>21611962</v>
+      </c>
+      <c r="AA2">
+        <v>9935434</v>
+      </c>
+      <c r="AB2">
+        <f>(Z2*4+AA2*64)/S2</f>
+        <v>14.550456499366828</v>
+      </c>
+      <c r="AD2">
+        <v>5713735</v>
+      </c>
+      <c r="AE2">
+        <f>(AA2*64+AD2*64)/S2</f>
+        <v>20.175340106290367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>38436527</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="2">F3-C3</f>
+        <v>11205601</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E10" si="3">D3/F3*100</f>
+        <v>22.572765212643585</v>
+      </c>
+      <c r="F3">
+        <v>49642128</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>44401432</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>5240696</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="1"/>
+        <v>10.556952755933429</v>
+      </c>
+      <c r="M3">
+        <v>49642128</v>
+      </c>
+      <c r="O3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3">
+        <v>8</v>
+      </c>
+      <c r="Q3">
+        <v>21611962</v>
+      </c>
+      <c r="R3">
+        <v>11205601</v>
+      </c>
+      <c r="S3" s="11">
+        <v>49642128</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T10" si="4">(R3*64 + Q3* 4)/S3</f>
+        <v>16.187990812964344</v>
+      </c>
+      <c r="U3">
+        <v>6151843</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V10" si="5">(R3*64 + U3 *64)/S3</f>
+        <v>22.377695331674744</v>
+      </c>
+      <c r="X3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y3">
+        <v>8</v>
+      </c>
+      <c r="Z3">
+        <v>21611962</v>
+      </c>
+      <c r="AA3">
+        <v>5240696</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB10" si="6">(Z3*4+AA3*64)/S3</f>
+        <v>8.4978708406698438</v>
+      </c>
+      <c r="AD3">
+        <v>2952328</v>
+      </c>
+      <c r="AE3">
+        <f t="shared" ref="AE3:AE10" si="7">(AA3*64+AD3*64)/S3</f>
+        <v>10.562672414043169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>43613016</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>6029112</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>12.14515219814912</v>
+      </c>
+      <c r="F4">
+        <v>49642128</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>46806123</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>2836005</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>5.7128997370942685</v>
+      </c>
+      <c r="M4">
+        <v>49642128</v>
+      </c>
+      <c r="O4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4">
+        <v>16</v>
+      </c>
+      <c r="Q4">
+        <v>21611962</v>
+      </c>
+      <c r="R4">
+        <v>6029112</v>
+      </c>
+      <c r="S4" s="11">
+        <v>49642128</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="4"/>
+        <v>9.5143184836878874</v>
+      </c>
+      <c r="U4">
+        <v>3186613</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="5"/>
+        <v>11.881166738057644</v>
+      </c>
+      <c r="X4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y4">
+        <v>16</v>
+      </c>
+      <c r="Z4">
+        <v>21611962</v>
+      </c>
+      <c r="AA4">
+        <v>2836005</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="6"/>
+        <v>5.3976769086127812</v>
+      </c>
+      <c r="AD4">
+        <v>1551938</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" si="7"/>
+        <v>5.6570570866744472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>46186104</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>3456024</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>6.9618772184786275</v>
+      </c>
+      <c r="F5">
+        <v>49642128</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>48051653</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>1590475</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>3.2038815902493143</v>
+      </c>
+      <c r="M5">
+        <v>49642128</v>
+      </c>
+      <c r="O5" t="s">
+        <v>43</v>
+      </c>
+      <c r="P5">
+        <v>32</v>
+      </c>
+      <c r="Q5">
+        <v>21611962</v>
+      </c>
+      <c r="R5">
+        <v>3456024</v>
+      </c>
+      <c r="S5" s="11">
+        <v>49642128</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="4"/>
+        <v>6.1970224966987715</v>
+      </c>
+      <c r="U5">
+        <v>1718195</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="5"/>
+        <v>6.6707457826948922</v>
+      </c>
+      <c r="X5" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y5">
+        <v>32</v>
+      </c>
+      <c r="Z5">
+        <v>21611962</v>
+      </c>
+      <c r="AA5">
+        <v>1590475</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="6"/>
+        <v>3.7919052946320111</v>
+      </c>
+      <c r="AD5">
+        <v>833638</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="7"/>
+        <v>3.1252333099016223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>64</v>
+      </c>
+      <c r="C6">
+        <v>47407327</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>2234801</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>4.5018235318195865</v>
+      </c>
+      <c r="F6">
+        <v>49642128</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6">
+        <v>64</v>
+      </c>
+      <c r="J6">
+        <v>48675572</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>966556</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>1.9470478783665357</v>
+      </c>
+      <c r="M6">
+        <v>49642128</v>
+      </c>
+      <c r="O6" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6">
+        <v>64</v>
+      </c>
+      <c r="Q6">
+        <v>21611962</v>
+      </c>
+      <c r="R6">
+        <v>2234801</v>
+      </c>
+      <c r="S6" s="11">
+        <v>49642128</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="4"/>
+        <v>4.6225881372369857</v>
+      </c>
+      <c r="U6">
+        <v>1013942</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="5"/>
+        <v>4.1883690401023905</v>
+      </c>
+      <c r="X6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y6">
+        <v>64</v>
+      </c>
+      <c r="Z6">
+        <v>21611962</v>
+      </c>
+      <c r="AA6">
+        <v>966556</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="6"/>
+        <v>2.9875317190270327</v>
+      </c>
+      <c r="AD6">
+        <v>469885</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="7"/>
+        <v>1.8518993384006424</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7">
+        <v>128</v>
+      </c>
+      <c r="C7">
+        <v>47825038</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>1817090</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>3.660378942659348</v>
+      </c>
+      <c r="F7">
+        <v>49642128</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7">
+        <v>128</v>
+      </c>
+      <c r="J7">
+        <v>48969562</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>672566</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>1.3548291080511294</v>
+      </c>
+      <c r="M7">
+        <v>49642128</v>
+      </c>
+      <c r="O7" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7">
+        <v>128</v>
+      </c>
+      <c r="Q7">
+        <v>21611962</v>
+      </c>
+      <c r="R7">
+        <v>1817090</v>
+      </c>
+      <c r="S7" s="11">
+        <v>49642128</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="4"/>
+        <v>4.0840636001744324</v>
+      </c>
+      <c r="U7">
+        <v>745650</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="5"/>
+        <v>3.3039550601054009</v>
+      </c>
+      <c r="X7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y7">
+        <v>128</v>
+      </c>
+      <c r="Z7">
+        <v>21611962</v>
+      </c>
+      <c r="AA7">
+        <v>672566</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="6"/>
+        <v>2.608511706025173</v>
+      </c>
+      <c r="AD7">
+        <v>292544</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="7"/>
+        <v>1.2442464190898506</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>256</v>
+      </c>
+      <c r="C8">
+        <v>47908952</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>1733176</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>3.4913410641864506</v>
+      </c>
+      <c r="F8">
+        <v>49642128</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8">
+        <v>256</v>
+      </c>
+      <c r="J8">
+        <v>49071087</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>571041</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>1.1503153128326811</v>
+      </c>
+      <c r="M8">
+        <v>49642128</v>
+      </c>
+      <c r="O8" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8">
+        <v>256</v>
+      </c>
+      <c r="Q8">
+        <v>21611962</v>
+      </c>
+      <c r="R8">
+        <v>1733176</v>
+      </c>
+      <c r="S8" s="11">
+        <v>49642128</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="4"/>
+        <v>3.9758793579517784</v>
+      </c>
+      <c r="U8">
+        <v>654014</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="5"/>
+        <v>3.0776311603724964</v>
+      </c>
+      <c r="X8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y8">
+        <v>256</v>
+      </c>
+      <c r="Z8">
+        <v>21611962</v>
+      </c>
+      <c r="AA8">
+        <v>571041</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="6"/>
+        <v>2.4776228770853659</v>
+      </c>
+      <c r="AD8">
+        <v>221558</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="7"/>
+        <v>1.0218404819390499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>512</v>
+      </c>
+      <c r="C9">
+        <v>47493475</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>2148653</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>4.3282854433637494</v>
+      </c>
+      <c r="F9">
+        <v>49642128</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9">
+        <v>512</v>
+      </c>
+      <c r="J9">
+        <v>48972332</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>669796</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>1.3492491699791758</v>
+      </c>
+      <c r="M9">
+        <v>49642128</v>
+      </c>
+      <c r="O9" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9">
+        <v>512</v>
+      </c>
+      <c r="Q9">
+        <v>21611962</v>
+      </c>
+      <c r="R9">
+        <v>2148653</v>
+      </c>
+      <c r="S9" s="11">
+        <v>49642128</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="4"/>
+        <v>4.5115237606252494</v>
+      </c>
+      <c r="U9">
+        <v>771170</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="5"/>
+        <v>3.7643163081163644</v>
+      </c>
+      <c r="X9" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y9">
+        <v>512</v>
+      </c>
+      <c r="Z9">
+        <v>21611962</v>
+      </c>
+      <c r="AA9">
+        <v>669796</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="6"/>
+        <v>2.6049405456591224</v>
+      </c>
+      <c r="AD9">
+        <v>247292</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="7"/>
+        <v>1.1823351327727127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>1024</v>
+      </c>
+      <c r="C10">
+        <v>46637378</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>3004750</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>6.0528227154162284</v>
+      </c>
+      <c r="F10">
+        <v>49642128</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10">
+        <v>1024</v>
+      </c>
+      <c r="J10">
+        <v>48679020</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>963108</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>1.9401021648387033</v>
+      </c>
+      <c r="M10">
+        <v>49642128</v>
+      </c>
+      <c r="O10" t="s">
+        <v>43</v>
+      </c>
+      <c r="P10">
+        <v>1024</v>
+      </c>
+      <c r="Q10">
+        <v>21611962</v>
+      </c>
+      <c r="R10">
+        <v>3004750</v>
+      </c>
+      <c r="S10" s="11">
+        <v>49642128</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="4"/>
+        <v>5.6152276147388367</v>
+      </c>
+      <c r="U10">
+        <v>1003517</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="5"/>
+        <v>5.1675683201977156</v>
+      </c>
+      <c r="X10" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y10">
+        <v>1024</v>
+      </c>
+      <c r="Z10">
+        <v>21611962</v>
+      </c>
+      <c r="AA10">
+        <v>963108</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="6"/>
+        <v>2.9830864623692199</v>
+      </c>
+      <c r="AD10">
+        <v>327111</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="7"/>
+        <v>1.6633859048105271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31">
+      <c r="S11" s="11"/>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="J16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="10:10">
+      <c r="J17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6">
+      <c r="F33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated stats.xlsx with Q6 and Q7
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>X - Log of cache size</t>
   </si>
@@ -140,24 +140,12 @@
     <t>Write Back</t>
   </si>
   <si>
-    <t>Total Data Traffic/Memory Op</t>
-  </si>
-  <si>
     <t>Write back Traffic</t>
   </si>
   <si>
     <t>Write through Traffic</t>
   </si>
   <si>
-    <t>Q:1 32 kb</t>
-  </si>
-  <si>
-    <t>Q:2 num of dirty evictions decrese with greater cache sizes</t>
-  </si>
-  <si>
-    <t>Q:3 num of dirty evictions increase with lesser cache size</t>
-  </si>
-  <si>
     <t>Hit - 2Way</t>
   </si>
   <si>
@@ -170,7 +158,22 @@
     <t>1- Way Miss Rate</t>
   </si>
   <si>
-    <t>Q:1  for lesser than 10%,</t>
+    <t>Q:1 At 32 kb, the two write policies generate approx same amount of traffice</t>
+  </si>
+  <si>
+    <t>Q:2 Number of dirty evictions decrease with greater cache sizes, thus decreasing the traffic for write back policy</t>
+  </si>
+  <si>
+    <t>Q:3 At smaller cache size, there are a large number of dirtly evictions, each eviction increases the traffic by a factor of 64(block size), therefore write back generates more traffic than write through at smaller cache sizes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q:1  for lesser than 10%, the cache should be 16 Kb. For lesser than 5%, cache should be 64 Kb </t>
+  </si>
+  <si>
+    <t>Q:2 4 MB</t>
+  </si>
+  <si>
+    <t>Q:3 As the cache size increases, the no. of blocks increases. This causes an improvement in hit rate in direct mapped cache. We see its not different from set assosciative, because at large cache sizes, …..</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFCD5B4"/>
+        <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -264,7 +267,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -316,8 +319,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -337,7 +342,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -353,8 +360,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -380,6 +389,7 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -405,6 +415,7 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -532,11 +543,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2125417160"/>
-        <c:axId val="-2123084424"/>
+        <c:axId val="2128737896"/>
+        <c:axId val="-2070442968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2125417160"/>
+        <c:axId val="2128737896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,12 +557,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123084424"/>
+        <c:crossAx val="-2070442968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123084424"/>
+        <c:axId val="-2070442968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,7 +573,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2125417160"/>
+        <c:crossAx val="2128737896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -876,11 +887,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127622216"/>
-        <c:axId val="-2123095976"/>
+        <c:axId val="-2069977704"/>
+        <c:axId val="-2069974712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2127622216"/>
+        <c:axId val="-2069977704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,12 +901,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123095976"/>
+        <c:crossAx val="-2069974712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123095976"/>
+        <c:axId val="-2069974712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,7 +917,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127622216"/>
+        <c:crossAx val="-2069977704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -953,7 +964,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Q6'!$M$1</c:f>
+              <c:f>'Q6'!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1000,7 +1011,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Q6'!$M$3:$M$11</c:f>
+              <c:f>'Q6'!$N$3:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1041,7 +1052,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Q6'!$N$1</c:f>
+              <c:f>'Q6'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1088,7 +1099,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Q6'!$N$3:$N$11</c:f>
+              <c:f>'Q6'!$I$3:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1132,11 +1143,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2123937368"/>
-        <c:axId val="-2124633128"/>
+        <c:axId val="-2071598120"/>
+        <c:axId val="-2034719480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2123937368"/>
+        <c:axId val="-2071598120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1146,12 +1157,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124633128"/>
+        <c:crossAx val="-2034719480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2124633128"/>
+        <c:axId val="-2034719480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,7 +1173,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123937368"/>
+        <c:crossAx val="-2071598120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1388,11 +1399,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2102666600"/>
-        <c:axId val="-2105117368"/>
+        <c:axId val="-2035205896"/>
+        <c:axId val="-2034312728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2102666600"/>
+        <c:axId val="-2035205896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1402,12 +1413,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105117368"/>
+        <c:crossAx val="-2034312728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2105117368"/>
+        <c:axId val="-2034312728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1418,7 +1429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2102666600"/>
+        <c:crossAx val="-2035205896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1509,16 +1520,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1384300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>2438400</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1092200</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1544,16 +1555,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1899,7 +1910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A12" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2357,7 +2368,6 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -2369,26 +2379,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView showRuler="0" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="23.1640625" customWidth="1"/>
     <col min="7" max="7" width="25.33203125" customWidth="1"/>
     <col min="8" max="8" width="23.83203125" customWidth="1"/>
-    <col min="9" max="9" width="27.6640625" customWidth="1"/>
-    <col min="10" max="10" width="23.1640625" customWidth="1"/>
-    <col min="11" max="11" width="23" customWidth="1"/>
-    <col min="12" max="12" width="34.6640625" customWidth="1"/>
-    <col min="13" max="13" width="26.6640625" customWidth="1"/>
-    <col min="14" max="14" width="21.5" customWidth="1"/>
+    <col min="9" max="10" width="27.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="34.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2398,7 +2408,7 @@
       <c r="B1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
@@ -2414,21 +2424,19 @@
         <v>30</v>
       </c>
       <c r="H1" s="16"/>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="18"/>
+      <c r="N1" s="12" t="s">
         <v>39</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -2438,10 +2446,10 @@
       <c r="H2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>36</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2476,23 +2484,20 @@
         <f>(G3+H3)/E3</f>
         <v>19.340777494470018</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>4676824</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <f>D3*64</f>
         <v>873669504</v>
       </c>
-      <c r="L3">
-        <f>J3*64</f>
+      <c r="M3">
+        <f>K3*64</f>
         <v>299316736</v>
       </c>
-      <c r="M3">
-        <f>(K3+L3)/E3</f>
+      <c r="N3">
+        <f>(L3+M3)/E3</f>
         <v>23.628846853624001</v>
-      </c>
-      <c r="N3">
-        <v>19.340777494470018</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2526,23 +2531,20 @@
         <f t="shared" ref="I4:I11" si="2">(G4+H4)/E4</f>
         <v>16.14527354669405</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>3789508</v>
       </c>
-      <c r="K4">
-        <f t="shared" ref="K4:K11" si="3">D4*64</f>
+      <c r="L4">
+        <f t="shared" ref="L4:L11" si="3">D4*64</f>
         <v>715037888</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L11" si="4">J4*64</f>
+      <c r="M4">
+        <f t="shared" ref="M4:M11" si="4">K4*64</f>
         <v>242528512</v>
       </c>
-      <c r="M4">
-        <f t="shared" ref="M4:M11" si="5">(K4+L4)/E4</f>
+      <c r="N4">
+        <f t="shared" ref="N4:N11" si="5">(L4+M4)/E4</f>
         <v>19.289390656258732</v>
-      </c>
-      <c r="N4">
-        <v>16.14527354669405</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -2576,23 +2578,20 @@
         <f t="shared" si="2"/>
         <v>13.550856482220102</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>3148608</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f t="shared" si="3"/>
         <v>586245504</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f t="shared" si="4"/>
         <v>201510912</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <f t="shared" si="5"/>
         <v>15.868707642831104</v>
-      </c>
-      <c r="N5">
-        <v>13.550856482220102</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -2627,23 +2626,20 @@
         <f t="shared" si="2"/>
         <v>7.2143197406847666</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1688401</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f t="shared" si="3"/>
         <v>271686336</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f t="shared" si="4"/>
         <v>108057664</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <f t="shared" si="5"/>
         <v>7.6496317804909575</v>
-      </c>
-      <c r="N6">
-        <v>7.2143197406847666</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -2678,23 +2674,20 @@
         <f t="shared" si="2"/>
         <v>5.8067862038468618</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1241321</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f t="shared" si="3"/>
         <v>201813376</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f t="shared" si="4"/>
         <v>79444544</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f t="shared" si="5"/>
         <v>5.665710382117382</v>
-      </c>
-      <c r="N7">
-        <v>5.8067862038468618</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -2729,23 +2722,20 @@
         <f t="shared" si="2"/>
         <v>4.6231631327327465</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>888405</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <f t="shared" si="3"/>
         <v>143055808</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="4"/>
         <v>56857920</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <f t="shared" si="5"/>
         <v>4.0270982742722072</v>
-      </c>
-      <c r="N8">
-        <v>4.6231631327327465</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -2780,23 +2770,20 @@
         <f t="shared" si="2"/>
         <v>2.7815067073675812</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>374593</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f t="shared" si="3"/>
         <v>51632064</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="4"/>
         <v>23973952</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <f t="shared" si="5"/>
         <v>1.5230212532387815</v>
-      </c>
-      <c r="N9">
-        <v>2.7815067073675812</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -2831,23 +2818,20 @@
         <f t="shared" si="2"/>
         <v>2.5092695462209034</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>323427</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <f t="shared" si="3"/>
         <v>38117632</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f t="shared" si="4"/>
         <v>20699328</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <f t="shared" si="5"/>
         <v>1.1848194742981204</v>
-      </c>
-      <c r="N10">
-        <v>2.5092695462209034</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -2882,53 +2866,44 @@
         <f t="shared" si="2"/>
         <v>2.2710937774464464</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>260065</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <f t="shared" si="3"/>
         <v>26294080</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <f t="shared" si="4"/>
         <v>16644160</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <f t="shared" si="5"/>
         <v>0.86495566829850645</v>
       </c>
-      <c r="N11">
-        <v>2.2710937774464464</v>
-      </c>
     </row>
     <row r="12" spans="1:14">
       <c r="C12" s="1"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="F20">
-        <f>A11*2</f>
-        <v>8388608</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2943,10 +2918,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J14"/>
+  <dimension ref="A2:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2959,7 +2934,7 @@
     <col min="9" max="9" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2967,7 +2942,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>9</v>
@@ -2979,16 +2954,16 @@
         <v>11</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>256</v>
       </c>
@@ -3021,7 +2996,7 @@
         <v>26.338741965292062</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>512</v>
       </c>
@@ -3054,7 +3029,7 @@
         <v>21.535436595304695</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>1024</v>
       </c>
@@ -3087,7 +3062,7 @@
         <v>17.326461105776932</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3120,7 +3095,7 @@
         <v>7.839792846914218</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -3153,7 +3128,7 @@
         <v>5.6712597010345727</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -3186,7 +3161,7 @@
         <v>3.9283650370507885</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -3219,7 +3194,7 @@
         <v>1.2502163485014179</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -3252,7 +3227,7 @@
         <v>0.93648684842841545</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -3285,14 +3260,23 @@
         <v>0.58992837696240585</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="J14" t="s">
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="1" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
add a graph to q6
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Q4" sheetId="1" r:id="rId1"/>
@@ -458,6 +458,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -562,11 +563,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2064810888"/>
-        <c:axId val="2064805144"/>
+        <c:axId val="2123653672"/>
+        <c:axId val="2123655592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2064810888"/>
+        <c:axId val="2123653672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -576,12 +577,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064805144"/>
+        <c:crossAx val="2123655592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064805144"/>
+        <c:axId val="2123655592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,13 +593,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064810888"/>
+        <c:crossAx val="2123653672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -905,11 +907,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2066574520"/>
-        <c:axId val="2066577512"/>
+        <c:axId val="2123913000"/>
+        <c:axId val="2123915992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2066574520"/>
+        <c:axId val="2123913000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -919,12 +921,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066577512"/>
+        <c:crossAx val="2123915992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2066577512"/>
+        <c:axId val="2123915992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -935,13 +937,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066574520"/>
+        <c:crossAx val="2123913000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -981,83 +984,83 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Q8'!$E$1</c:f>
+              <c:f>'Q6'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Miss Rate 8KB</c:v>
+                  <c:v>Total Data Traffic/Memory Op</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Q8'!$G$2:$G$10</c:f>
+              <c:f>'Q6'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.0</c:v>
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Q8'!$E$2:$E$10</c:f>
+              <c:f>'Q6'!$I$3:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>43.41334440779815</c:v>
+                  <c:v>19.34077749447002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.57276521264358</c:v>
+                  <c:v>16.14527354669405</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.14515219814912</c:v>
+                  <c:v>13.5508564822201</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.961877218478627</c:v>
+                  <c:v>7.214319740684766</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.501823531819586</c:v>
+                  <c:v>5.806786203846862</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.660378942659348</c:v>
+                  <c:v>4.623163132732746</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.491341064186451</c:v>
+                  <c:v>2.781506707367581</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.328285443363749</c:v>
+                  <c:v>2.509269546220903</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.052822715416228</c:v>
+                  <c:v>2.271093777446446</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1069,83 +1072,83 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Q8'!$L$1</c:f>
+              <c:f>'Q6'!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Miss Rate 32 KB</c:v>
+                  <c:v>Total Data Traffic/Memory Op</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Q8'!$G$2:$G$10</c:f>
+              <c:f>'Q6'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.0</c:v>
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Q8'!$L$2:$L$10</c:f>
+              <c:f>'Q6'!$M$3:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>20.01411784764747</c:v>
+                  <c:v>23.628846853624</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.55695275593343</c:v>
+                  <c:v>19.28939065625873</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.712899737094268</c:v>
+                  <c:v>15.8687076428311</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.203881590249314</c:v>
+                  <c:v>7.649631780490957</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.947047878366536</c:v>
+                  <c:v>5.665710382117382</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.354829108051129</c:v>
+                  <c:v>4.027098274272207</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.150315312832681</c:v>
+                  <c:v>1.523021253238781</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.349249169979176</c:v>
+                  <c:v>1.18481947429812</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.940102164838703</c:v>
+                  <c:v>0.864955668298506</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1160,11 +1163,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2066614728"/>
-        <c:axId val="2066617720"/>
+        <c:axId val="2123954040"/>
+        <c:axId val="2123841768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2066614728"/>
+        <c:axId val="2123954040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,12 +1177,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066617720"/>
+        <c:crossAx val="2123841768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2066617720"/>
+        <c:axId val="2123841768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1190,7 +1193,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066614728"/>
+        <c:crossAx val="2123954040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1237,11 +1240,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Q8'!$V$1</c:f>
+              <c:f>'Q8'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>total data traffic/memops write back  8KB</c:v>
+                  <c:v>Miss Rate 8KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1284,36 +1287,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Q8'!$V$2:$V$10</c:f>
+              <c:f>'Q8'!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>43.36844222310534</c:v>
+                  <c:v>43.41334440779815</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.37769533167474</c:v>
+                  <c:v>22.57276521264358</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.88116673805764</c:v>
+                  <c:v>12.14515219814912</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.670745782694892</c:v>
+                  <c:v>6.961877218478627</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.18836904010239</c:v>
+                  <c:v>4.501823531819586</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.303955060105401</c:v>
+                  <c:v>3.660378942659348</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.077631160372496</c:v>
+                  <c:v>3.491341064186451</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.764316308116364</c:v>
+                  <c:v>4.328285443363749</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.167568320197716</c:v>
+                  <c:v>6.052822715416228</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1325,11 +1328,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Q8'!$AE$1</c:f>
+              <c:f>'Q8'!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>total data traffic/memops write back 32KB</c:v>
+                  <c:v>Miss Rate 32 KB</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1372,36 +1375,36 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Q8'!$AE$2:$AE$10</c:f>
+              <c:f>'Q8'!$L$2:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>20.17534010629037</c:v>
+                  <c:v>20.01411784764747</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.56267241404317</c:v>
+                  <c:v>10.55695275593343</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.657057086674447</c:v>
+                  <c:v>5.712899737094268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.125233309901622</c:v>
+                  <c:v>3.203881590249314</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.851899338400642</c:v>
+                  <c:v>1.947047878366536</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.244246419089851</c:v>
+                  <c:v>1.354829108051129</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.02184048193905</c:v>
+                  <c:v>1.150315312832681</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.182335132772713</c:v>
+                  <c:v>1.349249169979176</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.663385904810527</c:v>
+                  <c:v>1.940102164838703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1416,11 +1419,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2074806984"/>
-        <c:axId val="2065597112"/>
+        <c:axId val="2123864232"/>
+        <c:axId val="2123867224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2074806984"/>
+        <c:axId val="2123864232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,12 +1433,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2065597112"/>
+        <c:crossAx val="2123867224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2065597112"/>
+        <c:axId val="2123867224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,7 +1449,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2074806984"/>
+        <c:crossAx val="2123864232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1493,6 +1496,261 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
+              <c:f>'Q8'!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total data traffic/memops write back  8KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8'!$V$2:$V$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>43.36844222310534</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.37769533167474</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.88116673805764</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.670745782694892</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.18836904010239</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.303955060105401</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.077631160372496</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.764316308116364</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.167568320197716</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q8'!$AE$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total data traffic/memops write back 32KB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q8'!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q8'!$AE$2:$AE$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>20.17534010629037</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.56267241404317</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.657057086674447</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.125233309901622</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.851899338400642</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.244246419089851</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.02184048193905</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.182335132772713</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.663385904810527</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2123759160"/>
+        <c:axId val="2123762152"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2123759160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2123762152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2123762152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2123759160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
               <c:f>'Q8'!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1672,11 +1930,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2066300776"/>
-        <c:axId val="2066263944"/>
+        <c:axId val="2124110088"/>
+        <c:axId val="2124113080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2066300776"/>
+        <c:axId val="2124110088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1686,12 +1944,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066263944"/>
+        <c:crossAx val="2124113080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2066263944"/>
+        <c:axId val="2124113080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1702,7 +1960,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066300776"/>
+        <c:crossAx val="2124110088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1790,6 +2048,41 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2208,7 +2501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B10"/>
     </sheetView>
   </sheetViews>
@@ -2680,8 +2973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3189,6 +3482,7 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3201,7 +3495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated correct CPI calculation
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Q4" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
   <si>
     <t>X - Log of cache size</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>CPI Latency 100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CPI = </t>
   </si>
   <si>
     <t>Q 5:</t>
@@ -302,12 +299,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -316,6 +307,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -328,8 +325,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -393,22 +392,21 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -420,8 +418,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -448,6 +447,7 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -474,6 +474,7 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,11 +602,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115721288"/>
-        <c:axId val="2115945320"/>
+        <c:axId val="2130204680"/>
+        <c:axId val="2130286152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115721288"/>
+        <c:axId val="2130204680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -615,12 +616,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115945320"/>
+        <c:crossAx val="2130286152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115945320"/>
+        <c:axId val="2130286152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +632,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115721288"/>
+        <c:crossAx val="2130204680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -730,31 +731,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.474909496224658</c:v>
+                  <c:v>3.474909496224658</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.025541753568662</c:v>
+                  <c:v>3.025541753568662</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.660701853877013</c:v>
+                  <c:v>2.660701853877013</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.769626374598607</c:v>
+                  <c:v>1.769626374598607</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.571691970980777</c:v>
+                  <c:v>1.571691970980777</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.405244976605354</c:v>
+                  <c:v>1.405244976605354</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.146262041788378</c:v>
+                  <c:v>1.146262041788378</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.107978691002126</c:v>
+                  <c:v>1.107978691002126</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.074485223518218</c:v>
+                  <c:v>1.074485223518218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -818,31 +819,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>8.59975865659909</c:v>
+                  <c:v>7.599758656599088</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.4014446761831</c:v>
+                  <c:v>6.4014446761831</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.428538277005369</c:v>
+                  <c:v>5.428538277005369</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.052336998929619</c:v>
+                  <c:v>3.052336998929619</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.524511922615404</c:v>
+                  <c:v>2.524511922615404</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.080653270947612</c:v>
+                  <c:v>2.080653270947611</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.390032111435674</c:v>
+                  <c:v>1.390032111435674</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.28794317600567</c:v>
+                  <c:v>1.28794317600567</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.198627262715249</c:v>
+                  <c:v>1.198627262715249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -906,31 +907,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>29.22400445847124</c:v>
+                  <c:v>28.22400445847124</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.28095928925529</c:v>
+                  <c:v>23.28095928925529</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.26772039264715</c:v>
+                  <c:v>19.26772039264715</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.46589012058468</c:v>
+                  <c:v>9.465890120584678</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.288611680788543</c:v>
+                  <c:v>7.288611680788542</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.457694742658897</c:v>
+                  <c:v>5.457694742658897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.608882459672156</c:v>
+                  <c:v>2.608882459672156</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.187765601023389</c:v>
+                  <c:v>2.187765601023389</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8193374587004</c:v>
+                  <c:v>1.8193374587004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -945,11 +946,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2129578168"/>
-        <c:axId val="2122205192"/>
+        <c:axId val="2116489064"/>
+        <c:axId val="2116492056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2129578168"/>
+        <c:axId val="2116489064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,12 +960,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122205192"/>
+        <c:crossAx val="2116492056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122205192"/>
+        <c:axId val="2116492056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,7 +976,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129578168"/>
+        <c:crossAx val="2116489064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1201,11 +1202,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2128921784"/>
-        <c:axId val="2122153448"/>
+        <c:axId val="2089365336"/>
+        <c:axId val="2089371416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2128921784"/>
+        <c:axId val="2089365336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,12 +1216,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122153448"/>
+        <c:crossAx val="2089371416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122153448"/>
+        <c:axId val="2089371416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128921784"/>
+        <c:crossAx val="2089365336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1457,11 +1458,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2128938024"/>
-        <c:axId val="2128669640"/>
+        <c:axId val="2125432136"/>
+        <c:axId val="2125349544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2128938024"/>
+        <c:axId val="2125432136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1471,12 +1472,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128669640"/>
+        <c:crossAx val="2125349544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128669640"/>
+        <c:axId val="2125349544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,7 +1488,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128938024"/>
+        <c:crossAx val="2125432136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1713,11 +1714,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2114608872"/>
-        <c:axId val="2124372328"/>
+        <c:axId val="2124671080"/>
+        <c:axId val="2125392584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2114608872"/>
+        <c:axId val="2124671080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,12 +1728,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124372328"/>
+        <c:crossAx val="2125392584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2124372328"/>
+        <c:axId val="2125392584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1743,7 +1744,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114608872"/>
+        <c:crossAx val="2124671080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1969,11 +1970,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2130334776"/>
-        <c:axId val="2130613480"/>
+        <c:axId val="2129607272"/>
+        <c:axId val="2128931384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2130334776"/>
+        <c:axId val="2129607272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1983,12 +1984,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130613480"/>
+        <c:crossAx val="2128931384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2130613480"/>
+        <c:axId val="2128931384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,14 +2000,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130334776"/>
+        <c:crossAx val="2129607272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2225,11 +2225,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116155160"/>
-        <c:axId val="2130226824"/>
+        <c:axId val="2124542648"/>
+        <c:axId val="2128761544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2116155160"/>
+        <c:axId val="2124542648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2239,12 +2239,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130226824"/>
+        <c:crossAx val="2128761544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2130226824"/>
+        <c:axId val="2128761544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,7 +2255,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116155160"/>
+        <c:crossAx val="2124542648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3068,8 +3068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B10"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3134,16 +3134,16 @@
         <v>13651086</v>
       </c>
       <c r="G2">
-        <f>(G$12+(E2/D2)+(F2/D2)*10)</f>
-        <v>4.4749094962246581</v>
+        <f>((E2/D2)+(F2/D2)*10)</f>
+        <v>3.4749094962246581</v>
       </c>
       <c r="H2">
-        <f>(G$12+(E2/D2)+(F2/D2)*25)</f>
-        <v>8.5997586565990893</v>
+        <f>((E2/D2)+(F2/D2)*25)</f>
+        <v>7.5997586565990884</v>
       </c>
       <c r="I2">
-        <f>(G$12+(E2/D2)+(F2/D2)*100)</f>
-        <v>29.224004458471239</v>
+        <f>((E2/D2)+(F2/D2)*100)</f>
+        <v>28.224004458471239</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3168,16 +3168,16 @@
         <v>11172467</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G10" si="2">(G$12+(E3/D3)+(F3/D3)*10)</f>
-        <v>4.0255417535686622</v>
+        <f t="shared" ref="G3:G10" si="2">((E3/D3)+(F3/D3)*10)</f>
+        <v>3.0255417535686622</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H10" si="3">(G$12+(E3/D3)+(F3/D3)*25)</f>
-        <v>7.4014446761831003</v>
+        <f t="shared" ref="H3:H10" si="3">((E3/D3)+(F3/D3)*25)</f>
+        <v>6.4014446761831003</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I10" si="4">(G$12+(E3/D3)+(F3/D3)*100)</f>
-        <v>24.280959289255286</v>
+        <f t="shared" ref="I3:I10" si="4">((E3/D3)+(F3/D3)*100)</f>
+        <v>23.280959289255286</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3203,15 +3203,15 @@
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>3.6607018538770135</v>
+        <v>2.6607018538770135</v>
       </c>
       <c r="H4">
         <f t="shared" si="3"/>
-        <v>6.4285382770053694</v>
+        <v>5.4285382770053694</v>
       </c>
       <c r="I4">
         <f t="shared" si="4"/>
-        <v>20.267720392647149</v>
+        <v>19.267720392647149</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3237,15 +3237,15 @@
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>2.7696263745986069</v>
+        <v>1.7696263745986069</v>
       </c>
       <c r="H5">
         <f t="shared" si="3"/>
-        <v>4.0523369989296185</v>
+        <v>3.052336998929619</v>
       </c>
       <c r="I5">
         <f t="shared" si="4"/>
-        <v>10.465890120584678</v>
+        <v>9.4658901205846782</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3271,15 +3271,15 @@
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>2.5716919709807766</v>
+        <v>1.5716919709807766</v>
       </c>
       <c r="H6">
         <f t="shared" si="3"/>
-        <v>3.524511922615404</v>
+        <v>2.524511922615404</v>
       </c>
       <c r="I6">
         <f t="shared" si="4"/>
-        <v>8.2886116807885433</v>
+        <v>7.2886116807885424</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3305,15 +3305,15 @@
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>2.4052449766053545</v>
+        <v>1.4052449766053543</v>
       </c>
       <c r="H7">
         <f t="shared" si="3"/>
-        <v>3.0806532709476118</v>
+        <v>2.0806532709476113</v>
       </c>
       <c r="I7">
         <f t="shared" si="4"/>
-        <v>6.4576947426588971</v>
+        <v>5.4576947426588971</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3339,15 +3339,15 @@
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>2.1462620417883778</v>
+        <v>1.1462620417883778</v>
       </c>
       <c r="H8">
         <f t="shared" si="3"/>
-        <v>2.3900321114356742</v>
+        <v>1.3900321114356742</v>
       </c>
       <c r="I8">
         <f t="shared" si="4"/>
-        <v>3.6088824596721558</v>
+        <v>2.6088824596721558</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3373,15 +3373,15 @@
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>2.1079786910021263</v>
+        <v>1.1079786910021263</v>
       </c>
       <c r="H9">
         <f t="shared" si="3"/>
-        <v>2.2879431760056699</v>
+        <v>1.2879431760056701</v>
       </c>
       <c r="I9">
         <f t="shared" si="4"/>
-        <v>3.187765601023389</v>
+        <v>2.187765601023389</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3407,72 +3407,68 @@
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>2.0744852235182183</v>
+        <v>1.0744852235182183</v>
       </c>
       <c r="H10">
         <f t="shared" si="3"/>
-        <v>2.1986272627152488</v>
+        <v>1.1986272627152486</v>
       </c>
       <c r="I10">
         <f t="shared" si="4"/>
-        <v>2.8193374587004003</v>
+        <v>1.8193374587004005</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="F12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="7">
-        <v>1</v>
-      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="10">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="9">
         <f>C6/C7</f>
         <v>1.4107317893727178</v>
       </c>
@@ -3485,37 +3481,37 @@
     </row>
     <row r="30" spans="1:10">
       <c r="F30" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I30" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="J30" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="30">
       <c r="F31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H31">
         <f>(G6/G7)</f>
-        <v>1.0692016804917466</v>
+        <v>1.1184469591754085</v>
       </c>
       <c r="I31">
         <f>(H6/H7)</f>
-        <v>1.1440793924631645</v>
+        <v>1.21332658250437</v>
       </c>
       <c r="J31">
         <f>(I6/I7)</f>
-        <v>1.2835248507543704</v>
+        <v>1.3354744126340883</v>
       </c>
     </row>
   </sheetData>
@@ -3540,7 +3536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A11" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -3562,54 +3558,54 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" s="16"/>
+      <c r="I1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="11"/>
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="14" t="s">
+      <c r="L1" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="18"/>
+      <c r="N1" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="J1" s="12"/>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="19"/>
-      <c r="N1" s="12" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3619,13 +3615,13 @@
       <c r="B3" s="1">
         <v>256</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>8</v>
       </c>
       <c r="D3">
         <v>13651086</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="10">
         <v>49642128</v>
       </c>
       <c r="F3">
@@ -3666,13 +3662,13 @@
       <c r="B4" s="1">
         <v>512</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>9</v>
       </c>
       <c r="D4">
         <v>11172467</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="10">
         <v>49642128</v>
       </c>
       <c r="F4">
@@ -3713,13 +3709,13 @@
       <c r="B5" s="1">
         <v>1024</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>10</v>
       </c>
       <c r="D5">
         <v>9160086</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="10">
         <v>49642128</v>
       </c>
       <c r="F5">
@@ -3761,13 +3757,13 @@
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>14</v>
       </c>
       <c r="D6">
         <v>4245099</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="10">
         <v>49642128</v>
       </c>
       <c r="F6">
@@ -3809,13 +3805,13 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>15</v>
       </c>
       <c r="D7">
         <v>3153334</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="10">
         <v>49642128</v>
       </c>
       <c r="F7">
@@ -3857,13 +3853,13 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>16</v>
       </c>
       <c r="D8">
         <v>2235247</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="10">
         <v>49642128</v>
       </c>
       <c r="F8">
@@ -3905,13 +3901,13 @@
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>20</v>
       </c>
       <c r="D9">
         <v>806751</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="10">
         <v>49642128</v>
       </c>
       <c r="F9">
@@ -3953,13 +3949,13 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>21</v>
       </c>
       <c r="D10">
         <v>595588</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="10">
         <v>49642128</v>
       </c>
       <c r="F10">
@@ -4001,13 +3997,13 @@
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>22</v>
       </c>
       <c r="D11">
         <v>410845</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="10">
         <v>49642128</v>
       </c>
       <c r="F11">
@@ -4046,17 +4042,17 @@
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -4079,7 +4075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I16"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A22" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
@@ -4101,7 +4097,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>9</v>
@@ -4113,13 +4109,13 @@
         <v>11</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4421,17 +4417,17 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4449,7 +4445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A17" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -4468,93 +4464,93 @@
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" t="s">
         <v>47</v>
       </c>
-      <c r="M1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>48</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>31</v>
+      </c>
+      <c r="T1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" t="s">
         <v>49</v>
       </c>
-      <c r="S1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>51</v>
       </c>
-      <c r="U1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" t="s">
         <v>52</v>
       </c>
-      <c r="X1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>53</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:31">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -4577,7 +4573,7 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2">
         <v>4</v>
@@ -4597,7 +4593,7 @@
         <v>49642128</v>
       </c>
       <c r="O2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P2">
         <v>4</v>
@@ -4608,7 +4604,7 @@
       <c r="R2">
         <v>21551308</v>
       </c>
-      <c r="S2" s="11">
+      <c r="S2" s="10">
         <v>49642128</v>
       </c>
       <c r="T2">
@@ -4623,7 +4619,7 @@
         <v>43.36844222310534</v>
       </c>
       <c r="X2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y2">
         <v>4</v>
@@ -4648,7 +4644,7 @@
     </row>
     <row r="3" spans="1:31">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -4671,7 +4667,7 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3">
         <v>8</v>
@@ -4691,7 +4687,7 @@
         <v>49642128</v>
       </c>
       <c r="O3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P3">
         <v>8</v>
@@ -4702,7 +4698,7 @@
       <c r="R3">
         <v>11205601</v>
       </c>
-      <c r="S3" s="11">
+      <c r="S3" s="10">
         <v>49642128</v>
       </c>
       <c r="T3">
@@ -4717,7 +4713,7 @@
         <v>22.377695331674744</v>
       </c>
       <c r="X3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y3">
         <v>8</v>
@@ -4742,7 +4738,7 @@
     </row>
     <row r="4" spans="1:31">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -4765,7 +4761,7 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4">
         <v>16</v>
@@ -4785,7 +4781,7 @@
         <v>49642128</v>
       </c>
       <c r="O4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P4">
         <v>16</v>
@@ -4796,7 +4792,7 @@
       <c r="R4">
         <v>6029112</v>
       </c>
-      <c r="S4" s="11">
+      <c r="S4" s="10">
         <v>49642128</v>
       </c>
       <c r="T4">
@@ -4811,7 +4807,7 @@
         <v>11.881166738057644</v>
       </c>
       <c r="X4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y4">
         <v>16</v>
@@ -4836,7 +4832,7 @@
     </row>
     <row r="5" spans="1:31">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>32</v>
@@ -4859,7 +4855,7 @@
         <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I5">
         <v>32</v>
@@ -4879,7 +4875,7 @@
         <v>49642128</v>
       </c>
       <c r="O5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P5">
         <v>32</v>
@@ -4890,7 +4886,7 @@
       <c r="R5">
         <v>3456024</v>
       </c>
-      <c r="S5" s="11">
+      <c r="S5" s="10">
         <v>49642128</v>
       </c>
       <c r="T5">
@@ -4905,7 +4901,7 @@
         <v>6.6707457826948922</v>
       </c>
       <c r="X5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y5">
         <v>32</v>
@@ -4930,7 +4926,7 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>64</v>
@@ -4953,7 +4949,7 @@
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I6">
         <v>64</v>
@@ -4973,7 +4969,7 @@
         <v>49642128</v>
       </c>
       <c r="O6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P6">
         <v>64</v>
@@ -4984,7 +4980,7 @@
       <c r="R6">
         <v>2234801</v>
       </c>
-      <c r="S6" s="11">
+      <c r="S6" s="10">
         <v>49642128</v>
       </c>
       <c r="T6">
@@ -4999,7 +4995,7 @@
         <v>4.1883690401023905</v>
       </c>
       <c r="X6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y6">
         <v>64</v>
@@ -5024,7 +5020,7 @@
     </row>
     <row r="7" spans="1:31">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>128</v>
@@ -5047,7 +5043,7 @@
         <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7">
         <v>128</v>
@@ -5067,7 +5063,7 @@
         <v>49642128</v>
       </c>
       <c r="O7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P7">
         <v>128</v>
@@ -5078,7 +5074,7 @@
       <c r="R7">
         <v>1817090</v>
       </c>
-      <c r="S7" s="11">
+      <c r="S7" s="10">
         <v>49642128</v>
       </c>
       <c r="T7">
@@ -5093,7 +5089,7 @@
         <v>3.3039550601054009</v>
       </c>
       <c r="X7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y7">
         <v>128</v>
@@ -5118,7 +5114,7 @@
     </row>
     <row r="8" spans="1:31">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>256</v>
@@ -5141,7 +5137,7 @@
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8">
         <v>256</v>
@@ -5161,7 +5157,7 @@
         <v>49642128</v>
       </c>
       <c r="O8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P8">
         <v>256</v>
@@ -5172,7 +5168,7 @@
       <c r="R8">
         <v>1733176</v>
       </c>
-      <c r="S8" s="11">
+      <c r="S8" s="10">
         <v>49642128</v>
       </c>
       <c r="T8">
@@ -5187,7 +5183,7 @@
         <v>3.0776311603724964</v>
       </c>
       <c r="X8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y8">
         <v>256</v>
@@ -5212,7 +5208,7 @@
     </row>
     <row r="9" spans="1:31">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>512</v>
@@ -5235,7 +5231,7 @@
         <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9">
         <v>512</v>
@@ -5255,7 +5251,7 @@
         <v>49642128</v>
       </c>
       <c r="O9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P9">
         <v>512</v>
@@ -5266,7 +5262,7 @@
       <c r="R9">
         <v>2148653</v>
       </c>
-      <c r="S9" s="11">
+      <c r="S9" s="10">
         <v>49642128</v>
       </c>
       <c r="T9">
@@ -5281,7 +5277,7 @@
         <v>3.7643163081163644</v>
       </c>
       <c r="X9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y9">
         <v>512</v>
@@ -5306,7 +5302,7 @@
     </row>
     <row r="10" spans="1:31">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10">
         <v>1024</v>
@@ -5329,7 +5325,7 @@
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I10">
         <v>1024</v>
@@ -5349,7 +5345,7 @@
         <v>49642128</v>
       </c>
       <c r="O10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P10">
         <v>1024</v>
@@ -5360,7 +5356,7 @@
       <c r="R10">
         <v>3004750</v>
       </c>
-      <c r="S10" s="11">
+      <c r="S10" s="10">
         <v>49642128</v>
       </c>
       <c r="T10">
@@ -5375,7 +5371,7 @@
         <v>5.1675683201977156</v>
       </c>
       <c r="X10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y10">
         <v>1024</v>
@@ -5399,21 +5395,21 @@
       </c>
     </row>
     <row r="11" spans="1:31">
-      <c r="S11" s="11"/>
+      <c r="S11" s="10"/>
     </row>
     <row r="16" spans="1:31">
       <c r="J16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="10:10">
       <c r="J17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="6:6">
       <c r="F33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prefetching code and related stats. one graph left
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14200" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Q4" sheetId="1" r:id="rId1"/>
     <sheet name="Q6" sheetId="2" r:id="rId2"/>
     <sheet name="Q7" sheetId="5" r:id="rId3"/>
     <sheet name="Q8" sheetId="4" r:id="rId4"/>
+    <sheet name="Q9" sheetId="6" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="85">
   <si>
     <t>X - Log of cache size</t>
   </si>
@@ -235,6 +236,51 @@
   </si>
   <si>
     <t>Q:3 As the cache size increases, the no. of blocks increases. This causes an improvement in hit rate in direct mapped cache. We see its not different from set assosciative, because at large cache sizes, …..</t>
+  </si>
+  <si>
+    <t>Log block</t>
+  </si>
+  <si>
+    <t>numHit</t>
+  </si>
+  <si>
+    <t>numMisses</t>
+  </si>
+  <si>
+    <t>numDirtyEvictions</t>
+  </si>
+  <si>
+    <t>N=0</t>
+  </si>
+  <si>
+    <t>N=1</t>
+  </si>
+  <si>
+    <t>Total Memory accesses</t>
+  </si>
+  <si>
+    <t>N=2</t>
+  </si>
+  <si>
+    <t>N=3</t>
+  </si>
+  <si>
+    <t>numPrefMisses</t>
+  </si>
+  <si>
+    <t>miss rate (N=0)</t>
+  </si>
+  <si>
+    <t>miss rate(N=1)</t>
+  </si>
+  <si>
+    <t>miss rate (N=2)</t>
+  </si>
+  <si>
+    <t>numPrefHits</t>
+  </si>
+  <si>
+    <t>miss rate(N=3)</t>
   </si>
 </sst>
 </file>
@@ -281,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +364,30 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -328,7 +398,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -382,8 +452,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -420,8 +508,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -448,6 +555,15 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -474,6 +590,15 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,11 +726,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115721288"/>
-        <c:axId val="2115945320"/>
+        <c:axId val="700021576"/>
+        <c:axId val="700024504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2115721288"/>
+        <c:axId val="700021576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -615,12 +740,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115945320"/>
+        <c:crossAx val="700024504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2115945320"/>
+        <c:axId val="700024504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +756,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115721288"/>
+        <c:crossAx val="700021576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -945,11 +1070,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2129578168"/>
-        <c:axId val="2122205192"/>
+        <c:axId val="591981144"/>
+        <c:axId val="591984136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2129578168"/>
+        <c:axId val="591981144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,12 +1084,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122205192"/>
+        <c:crossAx val="591984136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122205192"/>
+        <c:axId val="591984136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -975,7 +1100,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129578168"/>
+        <c:crossAx val="591981144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1201,11 +1326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2128921784"/>
-        <c:axId val="2122153448"/>
+        <c:axId val="592024360"/>
+        <c:axId val="592027352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2128921784"/>
+        <c:axId val="592024360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1215,12 +1340,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122153448"/>
+        <c:crossAx val="592027352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2122153448"/>
+        <c:axId val="592027352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1356,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128921784"/>
+        <c:crossAx val="592024360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1457,11 +1582,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2128938024"/>
-        <c:axId val="2128669640"/>
+        <c:axId val="592062600"/>
+        <c:axId val="592065592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2128938024"/>
+        <c:axId val="592062600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1471,12 +1596,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128669640"/>
+        <c:crossAx val="592065592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2128669640"/>
+        <c:axId val="592065592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,7 +1612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2128938024"/>
+        <c:crossAx val="592062600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1713,11 +1838,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2114608872"/>
-        <c:axId val="2124372328"/>
+        <c:axId val="592101640"/>
+        <c:axId val="592104632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2114608872"/>
+        <c:axId val="592101640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,12 +1852,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124372328"/>
+        <c:crossAx val="592104632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2124372328"/>
+        <c:axId val="592104632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1743,7 +1868,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2114608872"/>
+        <c:crossAx val="592101640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1969,11 +2094,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2130334776"/>
-        <c:axId val="2130613480"/>
+        <c:axId val="592133864"/>
+        <c:axId val="592136856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2130334776"/>
+        <c:axId val="592133864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1983,12 +2108,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130613480"/>
+        <c:crossAx val="592136856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2130613480"/>
+        <c:axId val="592136856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1999,7 +2124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130334776"/>
+        <c:crossAx val="592133864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2225,11 +2350,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2116155160"/>
-        <c:axId val="2130226824"/>
+        <c:axId val="592165176"/>
+        <c:axId val="592168168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2116155160"/>
+        <c:axId val="592165176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2239,12 +2364,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2130226824"/>
+        <c:crossAx val="592168168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2130226824"/>
+        <c:axId val="592168168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2255,7 +2380,461 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2116155160"/>
+        <c:crossAx val="592165176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0746190416328583"/>
+          <c:y val="0.0495867768595041"/>
+          <c:w val="0.788716501148532"/>
+          <c:h val="0.894361944426368"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q9'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>miss rate (N=0)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q9'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q9'!$F$3:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>34.80926724172662</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.10276344317874</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.57583993981886</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.538910418989291</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.630400372844613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.009327078001168</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.971995882207145</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.121412764577699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.259955818171211</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q9'!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>miss rate(N=1)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q9'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q9'!$J$3:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12.24069806193643</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.50475741088295</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.69107061647317</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.259780241491662</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.60111186208617</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.32864771631063</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.418075792399552</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.977665018711527</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.732469486400744</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q9'!$O$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>miss rate (N=2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q9'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q9'!$O$3:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>9.748476133013476</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.253453276620212</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.029932560505867</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.903282631236115</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.384614293730519</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.277958914251218</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.449772660833557</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.029479880475712</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.062658796576972</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Q9'!$T$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>miss rate(N=3)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Q9'!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Q9'!$T$3:$T$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>7.703406671043594</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.25832067473014</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.497670929819931</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6389144317101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.282408763782246</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.292019552425311</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.53012376906969</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.276693295662104</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.488166341297859</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="727384072"/>
+        <c:axId val="727381224"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="727384072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="727381224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="727381224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="727384072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2503,6 +3082,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3068,8 +3682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B10"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3526,7 +4140,6 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3540,8 +4153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4065,7 +4678,6 @@
     <mergeCell ref="L1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -4079,8 +4691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I16"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4449,14 +5061,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView showRuler="0" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
     <col min="12" max="12" width="15.5" customWidth="1"/>
     <col min="13" max="13" width="12.5" customWidth="1"/>
     <col min="19" max="19" width="22.6640625" customWidth="1"/>
@@ -5426,4 +6039,853 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="11" max="12" width="16.83203125" customWidth="1"/>
+    <col min="16" max="16" width="17.5" customWidth="1"/>
+    <col min="17" max="17" width="20.33203125" customWidth="1"/>
+    <col min="21" max="21" width="19.5" customWidth="1"/>
+    <col min="22" max="22" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23">
+      <c r="D1" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="26"/>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T2" t="s">
+        <v>84</v>
+      </c>
+      <c r="U2" t="s">
+        <v>73</v>
+      </c>
+      <c r="V2" t="s">
+        <v>79</v>
+      </c>
+      <c r="W2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3">
+        <v>32768</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>32362067</v>
+      </c>
+      <c r="E3">
+        <f>49642128-D3</f>
+        <v>17280061</v>
+      </c>
+      <c r="F3">
+        <f xml:space="preserve"> E3/49642128 *100</f>
+        <v>34.809267241726623</v>
+      </c>
+      <c r="G3">
+        <v>10838950</v>
+      </c>
+      <c r="H3">
+        <v>43565585</v>
+      </c>
+      <c r="I3">
+        <f>49642128-H3</f>
+        <v>6076543</v>
+      </c>
+      <c r="J3">
+        <f xml:space="preserve"> I3/49642128*100</f>
+        <v>12.240698061936426</v>
+      </c>
+      <c r="K3">
+        <v>6351430</v>
+      </c>
+      <c r="L3">
+        <v>49642128</v>
+      </c>
+      <c r="M3">
+        <v>44802777</v>
+      </c>
+      <c r="N3">
+        <f>L3-M3</f>
+        <v>4839351</v>
+      </c>
+      <c r="O3">
+        <f>N3/L3*100</f>
+        <v>9.7484761330134759</v>
+      </c>
+      <c r="P3">
+        <v>6283754</v>
+      </c>
+      <c r="Q3">
+        <v>49642128</v>
+      </c>
+      <c r="R3">
+        <v>45817993</v>
+      </c>
+      <c r="S3">
+        <f>Q3-R3</f>
+        <v>3824135</v>
+      </c>
+      <c r="T3">
+        <f>S3/Q3*100</f>
+        <v>7.7034066710435942</v>
+      </c>
+      <c r="U3">
+        <v>6226744</v>
+      </c>
+      <c r="V3">
+        <v>7572971</v>
+      </c>
+      <c r="W3">
+        <v>3899434</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4">
+        <v>32768</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>40655531</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E11" si="0">49642128-D4</f>
+        <v>8986597</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F11" si="1" xml:space="preserve"> E4/49642128 *100</f>
+        <v>18.102763443178745</v>
+      </c>
+      <c r="G4">
+        <v>5484340</v>
+      </c>
+      <c r="H4">
+        <v>46413028</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I11" si="2">49642128-H4</f>
+        <v>3229100</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J11" si="3" xml:space="preserve"> I4/49642128*100</f>
+        <v>6.5047574108829496</v>
+      </c>
+      <c r="K4">
+        <v>3266680</v>
+      </c>
+      <c r="L4">
+        <v>49642128</v>
+      </c>
+      <c r="M4">
+        <v>47034202</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N11" si="4">L4-M4</f>
+        <v>2607926</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O11" si="5">N4/L4*100</f>
+        <v>5.2534532766202124</v>
+      </c>
+      <c r="P4">
+        <v>3255867</v>
+      </c>
+      <c r="Q4">
+        <v>49642128</v>
+      </c>
+      <c r="R4">
+        <v>47528207</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4:S11" si="6">Q4-R4</f>
+        <v>2113921</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T11" si="7">S4/Q4*100</f>
+        <v>4.2583206747301405</v>
+      </c>
+      <c r="U4">
+        <v>3236061</v>
+      </c>
+      <c r="V4">
+        <v>4130849</v>
+      </c>
+      <c r="W4">
+        <v>2210914</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5">
+        <v>32768</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>44392056</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>5250072</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>10.575839939818858</v>
+      </c>
+      <c r="G5">
+        <v>3020669</v>
+      </c>
+      <c r="H5">
+        <v>47809802</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>1832326</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>3.6910706164731697</v>
+      </c>
+      <c r="K5">
+        <v>1712767</v>
+      </c>
+      <c r="L5">
+        <v>49642128</v>
+      </c>
+      <c r="M5">
+        <v>48138005</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="4"/>
+        <v>1504123</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="5"/>
+        <v>3.0299325605058671</v>
+      </c>
+      <c r="P5">
+        <v>1727093</v>
+      </c>
+      <c r="Q5">
+        <v>49642128</v>
+      </c>
+      <c r="R5">
+        <v>48402231</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="6"/>
+        <v>1239897</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="7"/>
+        <v>2.4976709298199307</v>
+      </c>
+      <c r="U5">
+        <v>1720221</v>
+      </c>
+      <c r="V5">
+        <v>2396141</v>
+      </c>
+      <c r="W5">
+        <v>1323550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6">
+        <v>32768</v>
+      </c>
+      <c r="B6">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>46892495</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>2749633</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>5.5389104189892908</v>
+      </c>
+      <c r="G6">
+        <v>1475140</v>
+      </c>
+      <c r="H6">
+        <v>48520325</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>1121803</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>2.2597802414916623</v>
+      </c>
+      <c r="K6">
+        <v>937742</v>
+      </c>
+      <c r="L6">
+        <v>49642128</v>
+      </c>
+      <c r="M6">
+        <v>48697298</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>944830</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="5"/>
+        <v>1.9032826312361146</v>
+      </c>
+      <c r="P6">
+        <v>953712</v>
+      </c>
+      <c r="Q6">
+        <v>49642128</v>
+      </c>
+      <c r="R6">
+        <v>48828536</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="6"/>
+        <v>813592</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="7"/>
+        <v>1.6389144317100992</v>
+      </c>
+      <c r="U6">
+        <v>955923</v>
+      </c>
+      <c r="V6">
+        <v>1533850</v>
+      </c>
+      <c r="W6">
+        <v>906926</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7">
+        <v>32768</v>
+      </c>
+      <c r="B7">
+        <v>64</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>47839920</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1802208</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>3.6304003728446133</v>
+      </c>
+      <c r="G7">
+        <v>855492</v>
+      </c>
+      <c r="H7">
+        <v>48847302</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>794826</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>1.60111186208617</v>
+      </c>
+      <c r="K7">
+        <v>562073</v>
+      </c>
+      <c r="L7">
+        <v>49642128</v>
+      </c>
+      <c r="M7">
+        <v>48954776</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="4"/>
+        <v>687352</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="5"/>
+        <v>1.3846142937305186</v>
+      </c>
+      <c r="P7">
+        <v>563607</v>
+      </c>
+      <c r="Q7">
+        <v>49642128</v>
+      </c>
+      <c r="R7">
+        <v>49005513</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="6"/>
+        <v>636615</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="7"/>
+        <v>1.2824087637822457</v>
+      </c>
+      <c r="U7">
+        <v>579784</v>
+      </c>
+      <c r="V7">
+        <v>1174930</v>
+      </c>
+      <c r="W7">
+        <v>734915</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8">
+        <v>32768</v>
+      </c>
+      <c r="B8">
+        <v>128</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>48148234</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1493894</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>3.0093270780011685</v>
+      </c>
+      <c r="G8">
+        <v>603538</v>
+      </c>
+      <c r="H8">
+        <v>48982559</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>659569</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>1.3286477163106305</v>
+      </c>
+      <c r="K8">
+        <v>363909</v>
+      </c>
+      <c r="L8">
+        <v>49642128</v>
+      </c>
+      <c r="M8">
+        <v>49007722</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>634406</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>1.2779589142512182</v>
+      </c>
+      <c r="P8">
+        <v>389990</v>
+      </c>
+      <c r="Q8">
+        <v>49642128</v>
+      </c>
+      <c r="R8">
+        <v>49000742</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="6"/>
+        <v>641386</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="7"/>
+        <v>1.2920195524253111</v>
+      </c>
+      <c r="U8">
+        <v>411128</v>
+      </c>
+      <c r="V8">
+        <v>1123432</v>
+      </c>
+      <c r="W8">
+        <v>800726</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9">
+        <v>32768</v>
+      </c>
+      <c r="B9">
+        <v>256</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>48166766</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1475362</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>2.9719958822071448</v>
+      </c>
+      <c r="G9">
+        <v>522546</v>
+      </c>
+      <c r="H9">
+        <v>48938165</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>703963</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>1.4180757923995524</v>
+      </c>
+      <c r="K9">
+        <v>314018</v>
+      </c>
+      <c r="L9">
+        <v>49642128</v>
+      </c>
+      <c r="M9">
+        <v>48922430</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="4"/>
+        <v>719698</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="5"/>
+        <v>1.4497726608335566</v>
+      </c>
+      <c r="P9">
+        <v>343518</v>
+      </c>
+      <c r="Q9">
+        <v>49642128</v>
+      </c>
+      <c r="R9">
+        <v>48882542</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="6"/>
+        <v>759586</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="7"/>
+        <v>1.5301237690696901</v>
+      </c>
+      <c r="U9">
+        <v>375098</v>
+      </c>
+      <c r="V9">
+        <v>1372112</v>
+      </c>
+      <c r="W9">
+        <v>906646</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10">
+        <v>32768</v>
+      </c>
+      <c r="B10">
+        <v>512</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>47596171</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>2045957</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>4.1214127645776992</v>
+      </c>
+      <c r="G10">
+        <v>683856</v>
+      </c>
+      <c r="H10">
+        <v>48660373</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>981755</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>1.9776650187115268</v>
+      </c>
+      <c r="K10">
+        <v>392997</v>
+      </c>
+      <c r="L10">
+        <v>49642128</v>
+      </c>
+      <c r="M10">
+        <v>48634651</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>1007477</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="5"/>
+        <v>2.0294798804757122</v>
+      </c>
+      <c r="P10">
+        <v>411911</v>
+      </c>
+      <c r="Q10">
+        <v>49642128</v>
+      </c>
+      <c r="R10">
+        <v>48511929</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="6"/>
+        <v>1130199</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="7"/>
+        <v>2.2766932956621035</v>
+      </c>
+      <c r="U10">
+        <v>463548</v>
+      </c>
+      <c r="V10">
+        <v>2157510</v>
+      </c>
+      <c r="W10">
+        <v>1233087</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11">
+        <v>32768</v>
+      </c>
+      <c r="B11">
+        <v>1024</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>47030974</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>2611154</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>5.2599558181712114</v>
+      </c>
+      <c r="G11">
+        <v>771229</v>
+      </c>
+      <c r="H11">
+        <v>48285672</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>1356456</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>2.7324694864007442</v>
+      </c>
+      <c r="K11">
+        <v>427688</v>
+      </c>
+      <c r="L11">
+        <v>49642128</v>
+      </c>
+      <c r="M11">
+        <v>48121759</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="4"/>
+        <v>1520369</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="5"/>
+        <v>3.0626587965769718</v>
+      </c>
+      <c r="P11">
+        <v>495311</v>
+      </c>
+      <c r="Q11">
+        <v>49642128</v>
+      </c>
+      <c r="R11">
+        <v>47910528</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="6"/>
+        <v>1731600</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="7"/>
+        <v>3.488166341297859</v>
+      </c>
+      <c r="U11">
+        <v>574577</v>
+      </c>
+      <c r="V11">
+        <v>3488861</v>
+      </c>
+      <c r="W11">
+        <v>1705939</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="M1:P1"/>
+    <mergeCell ref="R1:U1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated sheet with correct calculation
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="98">
   <si>
     <t>X - Log of cache size</t>
   </si>
@@ -278,9 +278,6 @@
   </si>
   <si>
     <t>out of cache (numDirtyEvictions *64)</t>
-  </si>
-  <si>
-    <t>Total Traffic per memory op</t>
   </si>
   <si>
     <t>Write-Back Traffic</t>
@@ -446,8 +443,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -603,12 +606,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -621,8 +618,14 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -673,6 +676,9 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -723,6 +729,9 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -849,11 +858,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116079592"/>
-        <c:axId val="-2113857928"/>
+        <c:axId val="2125936232"/>
+        <c:axId val="2125938040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116079592"/>
+        <c:axId val="2125936232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,12 +872,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113857928"/>
+        <c:crossAx val="2125938040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2113857928"/>
+        <c:axId val="2125938040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -879,7 +888,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116079592"/>
+        <c:crossAx val="2125936232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1192,11 +1201,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2127292216"/>
-        <c:axId val="-2113547432"/>
+        <c:axId val="2124959336"/>
+        <c:axId val="2124962328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2127292216"/>
+        <c:axId val="2124959336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,12 +1215,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113547432"/>
+        <c:crossAx val="2124962328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2113547432"/>
+        <c:axId val="2124962328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1222,7 +1231,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127292216"/>
+        <c:crossAx val="2124959336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1447,11 +1456,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116752664"/>
-        <c:axId val="-2111557720"/>
+        <c:axId val="2125006728"/>
+        <c:axId val="2125009720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116752664"/>
+        <c:axId val="2125006728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1461,12 +1470,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111557720"/>
+        <c:crossAx val="2125009720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111557720"/>
+        <c:axId val="2125009720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1477,13 +1486,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116752664"/>
+        <c:crossAx val="2125006728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1702,11 +1712,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2113776264"/>
-        <c:axId val="-2110918056"/>
+        <c:axId val="2125045032"/>
+        <c:axId val="2125048024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2113776264"/>
+        <c:axId val="2125045032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1716,12 +1726,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110918056"/>
+        <c:crossAx val="2125048024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2110918056"/>
+        <c:axId val="2125048024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1732,7 +1742,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113776264"/>
+        <c:crossAx val="2125045032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1957,11 +1967,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2119304904"/>
-        <c:axId val="-2116744312"/>
+        <c:axId val="2125084248"/>
+        <c:axId val="2125087240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2119304904"/>
+        <c:axId val="2125084248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1971,12 +1981,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116744312"/>
+        <c:crossAx val="2125087240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2116744312"/>
+        <c:axId val="2125087240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1987,13 +1997,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119304904"/>
+        <c:crossAx val="2125084248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2085,31 +2096,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>43.36844222310534</c:v>
+                  <c:v>2.710527638944084</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.37769533167474</c:v>
+                  <c:v>2.797211916459343</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.88116673805764</c:v>
+                  <c:v>2.970291684514411</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.670745782694892</c:v>
+                  <c:v>3.335372891347446</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4.18836904010239</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.303955060105401</c:v>
+                  <c:v>6.607910120210802</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.077631160372496</c:v>
+                  <c:v>12.31052464148999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.764316308116364</c:v>
+                  <c:v>30.11453046493092</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.167568320197716</c:v>
+                  <c:v>82.68109312316345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2173,31 +2184,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>20.17534010629037</c:v>
+                  <c:v>1.260958756643148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.56267241404317</c:v>
+                  <c:v>1.320334051755396</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.657057086674447</c:v>
+                  <c:v>1.414264271668612</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.125233309901622</c:v>
+                  <c:v>1.562616654950811</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.851899338400642</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.244246419089851</c:v>
+                  <c:v>2.488492838179701</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.02184048193905</c:v>
+                  <c:v>4.087361927756199</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.182335132772713</c:v>
+                  <c:v>9.458681062181701</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.663385904810527</c:v>
+                  <c:v>26.61417447696843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2212,11 +2223,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116327928"/>
-        <c:axId val="-2111404744"/>
+        <c:axId val="2125116440"/>
+        <c:axId val="2125119432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116327928"/>
+        <c:axId val="2125116440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2226,12 +2237,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111404744"/>
+        <c:crossAx val="2125119432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2111404744"/>
+        <c:axId val="2125119432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,13 +2253,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116327928"/>
+        <c:crossAx val="2125116440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2467,11 +2479,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116429432"/>
-        <c:axId val="-2113185176"/>
+        <c:axId val="2125147656"/>
+        <c:axId val="2125150648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116429432"/>
+        <c:axId val="2125147656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2481,12 +2493,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113185176"/>
+        <c:crossAx val="2125150648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2113185176"/>
+        <c:axId val="2125150648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,13 +2509,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116429432"/>
+        <c:crossAx val="2125147656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2608,31 +2621,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>34.80926724172662</c:v>
+                  <c:v>20.01411784764747</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.10276344317874</c:v>
+                  <c:v>10.55695275593343</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.57583993981886</c:v>
+                  <c:v>5.712899737094268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.538910418989291</c:v>
+                  <c:v>3.203881590249314</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.630400372844613</c:v>
+                  <c:v>1.947047878366536</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.009327078001168</c:v>
+                  <c:v>1.354829108051129</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.971995882207145</c:v>
+                  <c:v>1.150315312832681</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.121412764577699</c:v>
+                  <c:v>1.349249169979176</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.259955818171211</c:v>
+                  <c:v>1.940102164838703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2699,31 +2712,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12.24069806193643</c:v>
+                  <c:v>12.99321012185457</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.50475741088295</c:v>
+                  <c:v>6.895800276732697</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.69107061647317</c:v>
+                  <c:v>3.778302976858688</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.259780241491662</c:v>
+                  <c:v>2.209838788538638</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.60111186208617</c:v>
+                  <c:v>1.420599858249429</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.32864771631063</c:v>
+                  <c:v>1.088128212392506</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.418075792399552</c:v>
+                  <c:v>1.060413848495778</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.977665018711527</c:v>
+                  <c:v>1.36258058880957</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.732469486400744</c:v>
+                  <c:v>2.079953139800937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2790,31 +2803,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>9.748476133013476</c:v>
+                  <c:v>9.22209660311097</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.253453276620212</c:v>
+                  <c:v>4.904080663101309</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.029932560505867</c:v>
+                  <c:v>2.797355907063452</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.903282631236115</c:v>
+                  <c:v>1.692669178081971</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.384614293730519</c:v>
+                  <c:v>1.163417088002352</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.277958914251218</c:v>
+                  <c:v>0.982264499217278</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.449772660833557</c:v>
+                  <c:v>1.03354956902734</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.029479880475712</c:v>
+                  <c:v>1.416661670909837</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.062658796576972</c:v>
+                  <c:v>2.192442274029832</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2881,31 +2894,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>7.703406671043594</c:v>
+                  <c:v>7.149234214939376</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.25832067473014</c:v>
+                  <c:v>3.912986969454653</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.497670929819931</c:v>
+                  <c:v>2.265752991088537</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6389144317101</c:v>
+                  <c:v>1.415038049940164</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.282408763782246</c:v>
+                  <c:v>1.030328514522987</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.292019552425311</c:v>
+                  <c:v>0.939002856605986</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.53012376906969</c:v>
+                  <c:v>1.035457222945801</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.276693295662104</c:v>
+                  <c:v>1.456982263129413</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.488166341297859</c:v>
+                  <c:v>2.296827404336897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2920,11 +2933,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2112777784"/>
-        <c:axId val="-2112839016"/>
+        <c:axId val="2125201768"/>
+        <c:axId val="2125204904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2112777784"/>
+        <c:axId val="2125201768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2934,12 +2947,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112839016"/>
+        <c:crossAx val="2125204904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112839016"/>
+        <c:axId val="2125204904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2950,7 +2963,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112777784"/>
+        <c:crossAx val="2125201768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3061,31 +3074,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>36.25180419340605</c:v>
+                  <c:v>1.260958756643148</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.65633092924622</c:v>
+                  <c:v>1.320334051755396</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.66286731302091</c:v>
+                  <c:v>1.414264271668612</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.446693824245406</c:v>
+                  <c:v>1.562616654950811</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.426380110054911</c:v>
+                  <c:v>1.851899338400642</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.704067158442522</c:v>
+                  <c:v>2.488492838179701</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.575758073868228</c:v>
+                  <c:v>4.087361927756199</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.519350177736136</c:v>
+                  <c:v>9.458681062181701</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.36066141241971</c:v>
+                  <c:v>26.61417447696843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3152,31 +3165,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>22.70866067627077</c:v>
+                  <c:v>1.261277679313022</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.94053695683634</c:v>
+                  <c:v>1.34215857950328</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.465806300648514</c:v>
+                  <c:v>1.451351158838316</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.746844696101666</c:v>
+                  <c:v>1.675360250471132</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.471035407668261</c:v>
+                  <c:v>2.11019994952674</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.850910500855241</c:v>
+                  <c:v>3.108683495598738</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.829955395949182</c:v>
+                  <c:v>5.834456089392461</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.479028618595883</c:v>
+                  <c:v>15.13337607122724</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.313339347579942</c:v>
+                  <c:v>45.79602421556143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3243,31 +3256,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>22.7086387594021</c:v>
+                  <c:v>1.269437764634103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.00961248075425</c:v>
+                  <c:v>1.34579291202021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.68930679200537</c:v>
+                  <c:v>1.512111487243254</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.01263314094835</c:v>
+                  <c:v>1.798349982095852</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.709997605259791</c:v>
+                  <c:v>2.38135673797062</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.273218907940449</c:v>
+                  <c:v>3.800158123761334</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.452082473176814</c:v>
+                  <c:v>7.767797222552587</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.431004569344811</c:v>
+                  <c:v>21.77312495548136</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.085033260459745</c:v>
+                  <c:v>67.27069814573622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3334,31 +3347,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>22.7211532914141</c:v>
+                  <c:v>1.26002922356592</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.22294870195734</c:v>
+                  <c:v>1.360947782093467</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.90543676935042</c:v>
+                  <c:v>1.551787465678345</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.258789228374739</c:v>
+                  <c:v>1.901211003686224</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.082967273280468</c:v>
+                  <c:v>2.642866236515888</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.805289571792732</c:v>
+                  <c:v>4.523110532247933</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.231830512986873</c:v>
+                  <c:v>9.842107655014306</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.836223942696413</c:v>
+                  <c:v>28.42120740674131</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.471122752836058</c:v>
+                  <c:v>91.42548022921177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3373,11 +3386,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2110320136"/>
-        <c:axId val="-2112221240"/>
+        <c:axId val="2125241768"/>
+        <c:axId val="2125244904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2110320136"/>
+        <c:axId val="2125241768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3387,12 +3400,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112221240"/>
+        <c:crossAx val="2125244904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2112221240"/>
+        <c:axId val="2125244904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3403,7 +3416,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110320136"/>
+        <c:crossAx val="2125241768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3665,14 +3678,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1790700</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>1854200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3695,14 +3708,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1270000</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>1892300</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4753,7 +4766,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5291,7 +5304,7 @@
   <dimension ref="A2:I16"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5660,8 +5673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showRuler="0" topLeftCell="S9" workbookViewId="0">
+      <selection activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5675,6 +5688,7 @@
     <col min="20" max="20" width="32.6640625" customWidth="1"/>
     <col min="21" max="21" width="13.83203125" customWidth="1"/>
     <col min="22" max="22" width="12.1640625" customWidth="1"/>
+    <col min="28" max="28" width="11.5" customWidth="1"/>
     <col min="30" max="30" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5734,13 +5748,13 @@
         <v>32</v>
       </c>
       <c r="T1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U1" t="s">
         <v>50</v>
       </c>
       <c r="V1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X1" t="s">
         <v>28</v>
@@ -5755,13 +5769,13 @@
         <v>49</v>
       </c>
       <c r="AB1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AD1" t="s">
         <v>50</v>
       </c>
       <c r="AE1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:31">
@@ -5831,8 +5845,8 @@
         <v>12087782</v>
       </c>
       <c r="V2">
-        <f>(R2*64 + U2 *64)/S2</f>
-        <v>43.36844222310534</v>
+        <f>(R2*Y2 + U2 *Y2)/S2</f>
+        <v>2.7105276389440838</v>
       </c>
       <c r="X2" t="s">
         <v>43</v>
@@ -5854,8 +5868,8 @@
         <v>5713735</v>
       </c>
       <c r="AE2">
-        <f>(AA2*64+AD2*64)/S2</f>
-        <v>20.175340106290367</v>
+        <f>(AA2*Y2+AD2*Y2)/S2</f>
+        <v>1.2609587566431479</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -5925,8 +5939,8 @@
         <v>6151843</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V10" si="5">(R3*64 + U3 *64)/S3</f>
-        <v>22.377695331674744</v>
+        <f t="shared" ref="V3:V10" si="5">(R3*Y3 + U3 *Y3)/S3</f>
+        <v>2.797211916459343</v>
       </c>
       <c r="X3" t="s">
         <v>43</v>
@@ -5948,8 +5962,8 @@
         <v>2952328</v>
       </c>
       <c r="AE3">
-        <f t="shared" ref="AE3:AE10" si="7">(AA3*64+AD3*64)/S3</f>
-        <v>10.562672414043169</v>
+        <f t="shared" ref="AE3:AE10" si="7">(AA3*Y3+AD3*Y3)/S3</f>
+        <v>1.3203340517553961</v>
       </c>
     </row>
     <row r="4" spans="1:31">
@@ -6020,7 +6034,7 @@
       </c>
       <c r="V4">
         <f t="shared" si="5"/>
-        <v>11.881166738057644</v>
+        <v>2.9702916845144109</v>
       </c>
       <c r="X4" t="s">
         <v>43</v>
@@ -6043,7 +6057,7 @@
       </c>
       <c r="AE4">
         <f t="shared" si="7"/>
-        <v>5.6570570866744472</v>
+        <v>1.4142642716686118</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -6114,7 +6128,7 @@
       </c>
       <c r="V5">
         <f t="shared" si="5"/>
-        <v>6.6707457826948922</v>
+        <v>3.3353728913474461</v>
       </c>
       <c r="X5" t="s">
         <v>43</v>
@@ -6137,7 +6151,7 @@
       </c>
       <c r="AE5">
         <f t="shared" si="7"/>
-        <v>3.1252333099016223</v>
+        <v>1.5626166549508111</v>
       </c>
     </row>
     <row r="6" spans="1:31">
@@ -6302,7 +6316,7 @@
       </c>
       <c r="V7">
         <f t="shared" si="5"/>
-        <v>3.3039550601054009</v>
+        <v>6.6079101202108017</v>
       </c>
       <c r="X7" t="s">
         <v>43</v>
@@ -6325,7 +6339,7 @@
       </c>
       <c r="AE7">
         <f t="shared" si="7"/>
-        <v>1.2442464190898506</v>
+        <v>2.4884928381797011</v>
       </c>
     </row>
     <row r="8" spans="1:31">
@@ -6396,7 +6410,7 @@
       </c>
       <c r="V8">
         <f t="shared" si="5"/>
-        <v>3.0776311603724964</v>
+        <v>12.310524641489986</v>
       </c>
       <c r="X8" t="s">
         <v>43</v>
@@ -6419,7 +6433,7 @@
       </c>
       <c r="AE8">
         <f t="shared" si="7"/>
-        <v>1.0218404819390499</v>
+        <v>4.0873619277561994</v>
       </c>
     </row>
     <row r="9" spans="1:31">
@@ -6490,7 +6504,7 @@
       </c>
       <c r="V9">
         <f t="shared" si="5"/>
-        <v>3.7643163081163644</v>
+        <v>30.114530464930915</v>
       </c>
       <c r="X9" t="s">
         <v>43</v>
@@ -6513,7 +6527,7 @@
       </c>
       <c r="AE9">
         <f t="shared" si="7"/>
-        <v>1.1823351327727127</v>
+        <v>9.4586810621817019</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -6584,7 +6598,7 @@
       </c>
       <c r="V10">
         <f t="shared" si="5"/>
-        <v>5.1675683201977156</v>
+        <v>82.68109312316345</v>
       </c>
       <c r="X10" t="s">
         <v>43</v>
@@ -6607,7 +6621,7 @@
       </c>
       <c r="AE10">
         <f t="shared" si="7"/>
-        <v>1.6633859048105271</v>
+        <v>26.614174476968433</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -6641,10 +6655,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT78"/>
+  <dimension ref="A1:AK68"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="AJ16" sqref="AJ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6674,50 +6688,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
       <c r="Q1" s="18"/>
       <c r="R1" s="18"/>
       <c r="S1" s="16"/>
-      <c r="T1" s="29" t="s">
+      <c r="T1" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
       <c r="AB1" s="20"/>
-      <c r="AC1" s="32" t="s">
+      <c r="AC1" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
       <c r="AG1" s="19"/>
       <c r="AH1" s="19"/>
-      <c r="AI1" s="27" t="s">
+      <c r="AI1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="32"/>
     </row>
     <row r="2" spans="1:37">
       <c r="D2" s="15"/>
@@ -6732,8 +6746,8 @@
       <c r="M2" s="18"/>
       <c r="N2" s="18"/>
       <c r="O2" s="18"/>
-      <c r="P2" s="30" t="s">
-        <v>85</v>
+      <c r="P2" s="28" t="s">
+        <v>84</v>
       </c>
       <c r="Q2" s="26"/>
       <c r="R2" s="26"/>
@@ -6743,8 +6757,8 @@
       <c r="V2" s="17"/>
       <c r="W2" s="17"/>
       <c r="X2" s="17"/>
-      <c r="Y2" s="29" t="s">
-        <v>85</v>
+      <c r="Y2" s="27" t="s">
+        <v>84</v>
       </c>
       <c r="Z2" s="26"/>
       <c r="AA2" s="26"/>
@@ -6782,13 +6796,13 @@
         <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I3" t="s">
         <v>83</v>
       </c>
       <c r="J3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K3" t="s">
         <v>67</v>
@@ -6812,7 +6826,7 @@
         <v>83</v>
       </c>
       <c r="R3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S3" t="s">
         <v>72</v>
@@ -6839,7 +6853,7 @@
         <v>83</v>
       </c>
       <c r="AA3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AB3" t="s">
         <v>72</v>
@@ -6869,7 +6883,7 @@
         <v>83</v>
       </c>
       <c r="AK3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:37">
@@ -6883,126 +6897,125 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>32362067</v>
+        <v>39706694</v>
       </c>
       <c r="E4">
-        <f>49642128-D4</f>
-        <v>17280061</v>
+        <v>9935434</v>
       </c>
       <c r="F4">
         <f xml:space="preserve"> E4/49642128 *100</f>
-        <v>34.809267241726623</v>
+        <v>20.014117847647466</v>
       </c>
       <c r="G4">
-        <v>10838950</v>
+        <v>5713735</v>
       </c>
       <c r="H4">
-        <f>E4*64</f>
-        <v>1105923904</v>
+        <f>E4*B4</f>
+        <v>39741736</v>
       </c>
       <c r="I4">
-        <f>G4*64</f>
-        <v>693692800</v>
+        <f>G4*B4</f>
+        <v>22854940</v>
       </c>
       <c r="J4">
         <f>(H4+I4)/S4</f>
-        <v>36.251804193406052</v>
+        <v>1.2609587566431479</v>
       </c>
       <c r="K4">
-        <v>43565585</v>
+        <v>43192022</v>
       </c>
       <c r="L4">
         <f>49642128-K4</f>
-        <v>6076543</v>
+        <v>6450106</v>
       </c>
       <c r="M4">
         <f xml:space="preserve"> L4/49642128*100</f>
-        <v>12.240698061936426</v>
+        <v>12.993210121854567</v>
       </c>
       <c r="N4">
-        <v>6351430</v>
+        <v>5460710</v>
       </c>
       <c r="O4">
-        <v>5186187</v>
+        <v>3742311</v>
       </c>
       <c r="P4">
-        <f>(L4+O4)*64</f>
-        <v>720814720</v>
+        <f>(L4+O4)*B4</f>
+        <v>40769668</v>
       </c>
       <c r="Q4">
-        <f>N4*64</f>
-        <v>406491520</v>
+        <f>N4*B4</f>
+        <v>21842840</v>
       </c>
       <c r="R4">
         <f>(P4+Q4)/S4</f>
-        <v>22.708660676270767</v>
+        <v>1.2612776793130223</v>
       </c>
       <c r="S4">
         <v>49642128</v>
       </c>
       <c r="T4">
-        <v>44802777</v>
+        <v>45064083</v>
       </c>
       <c r="U4">
         <f>S4-T4</f>
-        <v>4839351</v>
+        <v>4578045</v>
       </c>
       <c r="V4">
         <f>U4/S4*100</f>
-        <v>9.7484761330134759</v>
+        <v>9.2220966031109697</v>
       </c>
       <c r="W4">
-        <v>6283754</v>
+        <v>5362510</v>
       </c>
       <c r="X4">
-        <v>6491038</v>
+        <v>5813843</v>
       </c>
       <c r="Y4">
-        <f>(X4+U4)*64</f>
-        <v>725144896</v>
+        <f>(X4+U4)*B4</f>
+        <v>41567552</v>
       </c>
       <c r="Z4">
-        <f>W4*64</f>
-        <v>402160256</v>
+        <f>W4*B4</f>
+        <v>21450040</v>
       </c>
       <c r="AA4">
         <f>(Y4+Z4)/S4</f>
-        <v>22.708638759402096</v>
+        <v>1.2694377646341026</v>
       </c>
       <c r="AB4">
         <v>49642128</v>
       </c>
       <c r="AC4">
-        <v>45817993</v>
+        <v>46093096</v>
       </c>
       <c r="AD4">
         <f>AB4-AC4</f>
-        <v>3824135</v>
+        <v>3549032</v>
       </c>
       <c r="AE4">
         <f>AD4/AB4*100</f>
-        <v>7.7034066710435942</v>
+        <v>7.1492342149393764</v>
       </c>
       <c r="AF4">
-        <v>6226744</v>
+        <v>5241978</v>
       </c>
       <c r="AG4">
-        <v>7572971</v>
+        <v>6846623</v>
       </c>
       <c r="AH4">
         <v>3899434</v>
       </c>
       <c r="AI4">
-        <f>(AD4+AG4)*64</f>
-        <v>729414784</v>
+        <f>(AD4+AG4)*B4</f>
+        <v>41582620</v>
       </c>
       <c r="AJ4">
-        <f>AF4*64</f>
-        <v>398511616</v>
+        <f>AF4*B4</f>
+        <v>20967912</v>
       </c>
       <c r="AK4">
         <f>(AI4+AJ4)/AB4</f>
-        <v>22.721153291414097</v>
+        <v>1.2600292235659196</v>
       </c>
     </row>
     <row r="5" spans="1:37">
@@ -7016,126 +7029,125 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>40655531</v>
+        <v>44401432</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E12" si="0">49642128-D5</f>
-        <v>8986597</v>
+        <v>5240696</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F12" si="1" xml:space="preserve"> E5/49642128 *100</f>
-        <v>18.102763443178745</v>
+        <f t="shared" ref="F5:F12" si="0" xml:space="preserve"> E5/49642128 *100</f>
+        <v>10.556952755933429</v>
       </c>
       <c r="G5">
-        <v>5484340</v>
+        <v>2952328</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H12" si="2">E5*64</f>
-        <v>575142208</v>
+        <f t="shared" ref="H5:H12" si="1">E5*B5</f>
+        <v>41925568</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I12" si="3">G5*64</f>
-        <v>350997760</v>
+        <f t="shared" ref="I5:I12" si="2">G5*B5</f>
+        <v>23618624</v>
       </c>
       <c r="J5">
-        <f t="shared" ref="J5:J12" si="4">(H5+I5)/S5</f>
-        <v>18.656330929246224</v>
+        <f t="shared" ref="J5:J12" si="3">(H5+I5)/S5</f>
+        <v>1.3203340517553961</v>
       </c>
       <c r="K5">
-        <v>46413028</v>
+        <v>46218906</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L12" si="5">49642128-K5</f>
-        <v>3229100</v>
+        <f t="shared" ref="L5:L12" si="4">49642128-K5</f>
+        <v>3423222</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M5:M12" si="6" xml:space="preserve"> L5/49642128*100</f>
-        <v>6.5047574108829496</v>
+        <f t="shared" ref="M5:M12" si="5" xml:space="preserve"> L5/49642128*100</f>
+        <v>6.8958002767326967</v>
       </c>
       <c r="N5">
-        <v>3266680</v>
+        <v>2849755</v>
       </c>
       <c r="O5">
-        <v>2765996</v>
+        <v>2055474</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P5:P12" si="7">(L5+O5)*64</f>
-        <v>383686144</v>
+        <f t="shared" ref="P5:P12" si="6">(L5+O5)*B5</f>
+        <v>43829568</v>
       </c>
       <c r="Q5">
-        <f t="shared" ref="Q5:Q12" si="8">N5*64</f>
-        <v>209067520</v>
+        <f t="shared" ref="Q5:Q12" si="7">N5*B5</f>
+        <v>22798040</v>
       </c>
       <c r="R5">
-        <f t="shared" ref="R5:R12" si="9">(P5+Q5)/S5</f>
-        <v>11.940536956836338</v>
+        <f t="shared" ref="R5:R12" si="8">(P5+Q5)/S5</f>
+        <v>1.34215857950328</v>
       </c>
       <c r="S5">
         <v>49642128</v>
       </c>
       <c r="T5">
-        <v>47034202</v>
+        <v>47207638</v>
       </c>
       <c r="U5">
-        <f t="shared" ref="U5:U12" si="10">S5-T5</f>
-        <v>2607926</v>
+        <f t="shared" ref="U5:U12" si="9">S5-T5</f>
+        <v>2434490</v>
       </c>
       <c r="V5">
-        <f t="shared" ref="V5:V12" si="11">U5/S5*100</f>
-        <v>5.2534532766202124</v>
+        <f t="shared" ref="V5:V12" si="10">U5/S5*100</f>
+        <v>4.9040806631013085</v>
       </c>
       <c r="W5">
-        <v>3255867</v>
+        <v>2790184</v>
       </c>
       <c r="X5">
-        <v>3451562</v>
+        <v>3126329</v>
       </c>
       <c r="Y5">
-        <f t="shared" ref="Y5:Y12" si="12">(X5+U5)*64</f>
-        <v>387807232</v>
+        <f t="shared" ref="Y5:Y12" si="11">(X5+U5)*B5</f>
+        <v>44486552</v>
       </c>
       <c r="Z5">
-        <f t="shared" ref="Z5:Z12" si="13">W5*64</f>
-        <v>208375488</v>
+        <f t="shared" ref="Z5:Z12" si="12">W5*B5</f>
+        <v>22321472</v>
       </c>
       <c r="AA5">
-        <f t="shared" ref="AA5:AA12" si="14">(Y5+Z5)/S5</f>
-        <v>12.009612480754249</v>
+        <f t="shared" ref="AA5:AA12" si="13">(Y5+Z5)/S5</f>
+        <v>1.3457929120202099</v>
       </c>
       <c r="AB5">
         <v>49642128</v>
       </c>
       <c r="AC5">
-        <v>47528207</v>
+        <v>47699638</v>
       </c>
       <c r="AD5">
-        <f t="shared" ref="AD5:AD12" si="15">AB5-AC5</f>
-        <v>2113921</v>
+        <f t="shared" ref="AD5:AD12" si="14">AB5-AC5</f>
+        <v>1942490</v>
       </c>
       <c r="AE5">
-        <f t="shared" ref="AE5:AE12" si="16">AD5/AB5*100</f>
-        <v>4.2583206747301405</v>
+        <f t="shared" ref="AE5:AE12" si="15">AD5/AB5*100</f>
+        <v>3.9129869694546535</v>
       </c>
       <c r="AF5">
-        <v>3236061</v>
+        <v>2734009</v>
       </c>
       <c r="AG5">
-        <v>4130849</v>
+        <v>3768544</v>
       </c>
       <c r="AH5">
         <v>2210914</v>
       </c>
       <c r="AI5">
-        <f t="shared" ref="AI5:AI12" si="17">(AD5+AG5)*64</f>
-        <v>399665280</v>
+        <f t="shared" ref="AI5:AI12" si="16">(AD5+AG5)*B5</f>
+        <v>45688272</v>
       </c>
       <c r="AJ5">
-        <f t="shared" ref="AJ5:AJ12" si="18">AF5*64</f>
-        <v>207107904</v>
+        <f t="shared" ref="AJ5:AJ12" si="17">AF5*B5</f>
+        <v>21872072</v>
       </c>
       <c r="AK5">
-        <f t="shared" ref="AK5:AK12" si="19">(AI5+AJ5)/AB5</f>
-        <v>12.222948701957337</v>
+        <f t="shared" ref="AK5:AK12" si="18">(AI5+AJ5)/AB5</f>
+        <v>1.360947782093467</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -7149,126 +7161,125 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>44392056</v>
+        <v>46806123</v>
       </c>
       <c r="E6">
+        <v>2836005</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="0"/>
-        <v>5250072</v>
-      </c>
-      <c r="F6">
+        <v>5.7128997370942685</v>
+      </c>
+      <c r="G6">
+        <v>1551938</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="1"/>
-        <v>10.575839939818858</v>
-      </c>
-      <c r="G6">
-        <v>3020669</v>
-      </c>
-      <c r="H6">
+        <v>45376080</v>
+      </c>
+      <c r="I6">
         <f t="shared" si="2"/>
-        <v>336004608</v>
-      </c>
-      <c r="I6">
+        <v>24831008</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="3"/>
-        <v>193322816</v>
-      </c>
-      <c r="J6">
+        <v>1.4142642716686118</v>
+      </c>
+      <c r="K6">
+        <v>47766498</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="4"/>
-        <v>10.662867313020909</v>
-      </c>
-      <c r="K6">
-        <v>47809802</v>
-      </c>
-      <c r="L6">
+        <v>1875630</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="5"/>
-        <v>1832326</v>
-      </c>
-      <c r="M6">
+        <v>3.7783029768586878</v>
+      </c>
+      <c r="N6">
+        <v>1495694</v>
+      </c>
+      <c r="O6">
+        <v>1131686</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="6"/>
-        <v>3.6910706164731697</v>
-      </c>
-      <c r="N6">
-        <v>1712767</v>
-      </c>
-      <c r="O6">
-        <v>1470163</v>
-      </c>
-      <c r="P6">
+        <v>48117056</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="7"/>
-        <v>211359296</v>
-      </c>
-      <c r="Q6">
+        <v>23931104</v>
+      </c>
+      <c r="R6">
         <f t="shared" si="8"/>
-        <v>109617088</v>
-      </c>
-      <c r="R6">
-        <f t="shared" si="9"/>
-        <v>6.4658063006485138</v>
+        <v>1.4513511588383157</v>
       </c>
       <c r="S6">
         <v>49642128</v>
       </c>
       <c r="T6">
-        <v>48138005</v>
+        <v>48253461</v>
       </c>
       <c r="U6">
+        <f t="shared" si="9"/>
+        <v>1388667</v>
+      </c>
+      <c r="V6">
         <f t="shared" si="10"/>
-        <v>1504123</v>
-      </c>
-      <c r="V6">
+        <v>2.7973559070634519</v>
+      </c>
+      <c r="W6">
+        <v>1496558</v>
+      </c>
+      <c r="X6">
+        <v>1806302</v>
+      </c>
+      <c r="Y6">
         <f t="shared" si="11"/>
-        <v>3.0299325605058671</v>
-      </c>
-      <c r="W6">
-        <v>1727093</v>
-      </c>
-      <c r="X6">
-        <v>1957400</v>
-      </c>
-      <c r="Y6">
+        <v>51119504</v>
+      </c>
+      <c r="Z6">
         <f t="shared" si="12"/>
-        <v>221537472</v>
-      </c>
-      <c r="Z6">
+        <v>23944928</v>
+      </c>
+      <c r="AA6">
         <f t="shared" si="13"/>
-        <v>110533952</v>
-      </c>
-      <c r="AA6">
-        <f t="shared" si="14"/>
-        <v>6.6893067920053708</v>
+        <v>1.5121114872432544</v>
       </c>
       <c r="AB6">
         <v>49642128</v>
       </c>
       <c r="AC6">
-        <v>48402231</v>
+        <v>48517360</v>
       </c>
       <c r="AD6">
+        <f t="shared" si="14"/>
+        <v>1124768</v>
+      </c>
+      <c r="AE6">
         <f t="shared" si="15"/>
-        <v>1239897</v>
-      </c>
-      <c r="AE6">
-        <f t="shared" si="16"/>
-        <v>2.4976709298199307</v>
+        <v>2.2657529910885366</v>
       </c>
       <c r="AF6">
-        <v>1720221</v>
+        <v>1481599</v>
       </c>
       <c r="AG6">
-        <v>2396141</v>
+        <v>2208260</v>
       </c>
       <c r="AH6">
         <v>1323550</v>
       </c>
       <c r="AI6">
+        <f t="shared" si="16"/>
+        <v>53328448</v>
+      </c>
+      <c r="AJ6">
         <f t="shared" si="17"/>
-        <v>232706432</v>
-      </c>
-      <c r="AJ6">
+        <v>23705584</v>
+      </c>
+      <c r="AK6">
         <f t="shared" si="18"/>
-        <v>110094144</v>
-      </c>
-      <c r="AK6">
-        <f t="shared" si="19"/>
-        <v>6.9054367693504197</v>
+        <v>1.5517874656783448</v>
       </c>
     </row>
     <row r="7" spans="1:37">
@@ -7282,126 +7293,125 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>46892495</v>
+        <v>48051653</v>
       </c>
       <c r="E7">
+        <v>1590475</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="0"/>
-        <v>2749633</v>
-      </c>
-      <c r="F7">
+        <v>3.2038815902493143</v>
+      </c>
+      <c r="G7">
+        <v>833638</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="1"/>
-        <v>5.5389104189892908</v>
-      </c>
-      <c r="G7">
-        <v>1475140</v>
-      </c>
-      <c r="H7">
+        <v>50895200</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="2"/>
-        <v>175976512</v>
-      </c>
-      <c r="I7">
+        <v>26676416</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="3"/>
-        <v>94408960</v>
-      </c>
-      <c r="J7">
+        <v>1.5626166549508111</v>
+      </c>
+      <c r="K7">
+        <v>48545117</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="4"/>
-        <v>5.4466938242454068</v>
-      </c>
-      <c r="K7">
-        <v>48520325</v>
-      </c>
-      <c r="L7">
+        <v>1097011</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="5"/>
-        <v>1121803</v>
-      </c>
-      <c r="M7">
+        <v>2.2098387885386379</v>
+      </c>
+      <c r="N7">
+        <v>818190</v>
+      </c>
+      <c r="O7">
+        <v>683813</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="6"/>
-        <v>2.2597802414916623</v>
-      </c>
-      <c r="N7">
-        <v>937742</v>
-      </c>
-      <c r="O7">
-        <v>846726</v>
-      </c>
-      <c r="P7">
+        <v>56986368</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="7"/>
-        <v>125985856</v>
-      </c>
-      <c r="Q7">
+        <v>26182080</v>
+      </c>
+      <c r="R7">
         <f t="shared" si="8"/>
-        <v>60015488</v>
-      </c>
-      <c r="R7">
-        <f t="shared" si="9"/>
-        <v>3.7468446961016659</v>
+        <v>1.675360250471132</v>
       </c>
       <c r="S7">
         <v>49642128</v>
       </c>
       <c r="T7">
-        <v>48697298</v>
+        <v>48801851</v>
       </c>
       <c r="U7">
+        <f t="shared" si="9"/>
+        <v>840277</v>
+      </c>
+      <c r="V7">
         <f t="shared" si="10"/>
-        <v>944830</v>
-      </c>
-      <c r="V7">
+        <v>1.6926691780819711</v>
+      </c>
+      <c r="W7">
+        <v>821965</v>
+      </c>
+      <c r="X7">
+        <v>1127568</v>
+      </c>
+      <c r="Y7">
         <f t="shared" si="11"/>
-        <v>1.9032826312361146</v>
-      </c>
-      <c r="W7">
-        <v>953712</v>
-      </c>
-      <c r="X7">
-        <v>1213890</v>
-      </c>
-      <c r="Y7">
+        <v>62971040</v>
+      </c>
+      <c r="Z7">
         <f t="shared" si="12"/>
-        <v>138158080</v>
-      </c>
-      <c r="Z7">
+        <v>26302880</v>
+      </c>
+      <c r="AA7">
         <f t="shared" si="13"/>
-        <v>61037568</v>
-      </c>
-      <c r="AA7">
-        <f t="shared" si="14"/>
-        <v>4.0126331409483491</v>
+        <v>1.7983499820958522</v>
       </c>
       <c r="AB7">
         <v>49642128</v>
       </c>
       <c r="AC7">
-        <v>48828536</v>
+        <v>48939673</v>
       </c>
       <c r="AD7">
+        <f t="shared" si="14"/>
+        <v>702455</v>
+      </c>
+      <c r="AE7">
         <f t="shared" si="15"/>
-        <v>813592</v>
-      </c>
-      <c r="AE7">
-        <f t="shared" si="16"/>
-        <v>1.6389144317100992</v>
+        <v>1.4150380499401638</v>
       </c>
       <c r="AF7">
-        <v>955923</v>
+        <v>825521</v>
       </c>
       <c r="AG7">
-        <v>1533850</v>
+        <v>1421404</v>
       </c>
       <c r="AH7">
         <v>906926</v>
       </c>
       <c r="AI7">
+        <f t="shared" si="16"/>
+        <v>67963488</v>
+      </c>
+      <c r="AJ7">
         <f t="shared" si="17"/>
-        <v>150236288</v>
-      </c>
-      <c r="AJ7">
+        <v>26416672</v>
+      </c>
+      <c r="AK7">
         <f t="shared" si="18"/>
-        <v>61179072</v>
-      </c>
-      <c r="AK7">
-        <f t="shared" si="19"/>
-        <v>4.2587892283747388</v>
+        <v>1.901211003686224</v>
       </c>
     </row>
     <row r="8" spans="1:37">
@@ -7415,126 +7425,125 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>47839920</v>
+        <v>48675572</v>
       </c>
       <c r="E8">
+        <v>966556</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="0"/>
-        <v>1802208</v>
-      </c>
-      <c r="F8">
+        <v>1.9470478783665357</v>
+      </c>
+      <c r="G8">
+        <v>469885</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="1"/>
-        <v>3.6304003728446133</v>
-      </c>
-      <c r="G8">
-        <v>855492</v>
-      </c>
-      <c r="H8">
+        <v>61859584</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="2"/>
-        <v>115341312</v>
-      </c>
-      <c r="I8">
+        <v>30072640</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="3"/>
-        <v>54751488</v>
-      </c>
-      <c r="J8">
+        <v>1.8518993384006424</v>
+      </c>
+      <c r="K8">
+        <v>48936912</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="4"/>
-        <v>3.4263801100549114</v>
-      </c>
-      <c r="K8">
-        <v>48847302</v>
-      </c>
-      <c r="L8">
+        <v>705216</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="5"/>
-        <v>794826</v>
-      </c>
-      <c r="M8">
+        <v>1.4205998582494288</v>
+      </c>
+      <c r="N8">
+        <v>469390</v>
+      </c>
+      <c r="O8">
+        <v>462188</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="6"/>
-        <v>1.60111186208617</v>
-      </c>
-      <c r="N8">
-        <v>562073</v>
-      </c>
-      <c r="O8">
-        <v>559780</v>
-      </c>
-      <c r="P8">
+        <v>74713856</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="7"/>
-        <v>86694784</v>
-      </c>
-      <c r="Q8">
+        <v>30040960</v>
+      </c>
+      <c r="R8">
         <f t="shared" si="8"/>
-        <v>35972672</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="9"/>
-        <v>2.471035407668261</v>
+        <v>2.1101999495267405</v>
       </c>
       <c r="S8">
         <v>49642128</v>
       </c>
       <c r="T8">
-        <v>48954776</v>
+        <v>49064583</v>
       </c>
       <c r="U8">
+        <f t="shared" si="9"/>
+        <v>577545</v>
+      </c>
+      <c r="V8">
         <f t="shared" si="10"/>
-        <v>687352</v>
-      </c>
-      <c r="V8">
+        <v>1.1634170880023516</v>
+      </c>
+      <c r="W8">
+        <v>479621</v>
+      </c>
+      <c r="X8">
+        <v>789953</v>
+      </c>
+      <c r="Y8">
         <f t="shared" si="11"/>
-        <v>1.3846142937305186</v>
-      </c>
-      <c r="W8">
-        <v>563607</v>
-      </c>
-      <c r="X8">
-        <v>851073</v>
-      </c>
-      <c r="Y8">
+        <v>87519872</v>
+      </c>
+      <c r="Z8">
         <f t="shared" si="12"/>
-        <v>98459200</v>
-      </c>
-      <c r="Z8">
+        <v>30695744</v>
+      </c>
+      <c r="AA8">
         <f t="shared" si="13"/>
-        <v>36070848</v>
-      </c>
-      <c r="AA8">
-        <f t="shared" si="14"/>
-        <v>2.7099976052597907</v>
+        <v>2.3813567379706204</v>
       </c>
       <c r="AB8">
         <v>49642128</v>
       </c>
       <c r="AC8">
-        <v>49005513</v>
+        <v>49130651</v>
       </c>
       <c r="AD8">
+        <f t="shared" si="14"/>
+        <v>511477</v>
+      </c>
+      <c r="AE8">
         <f t="shared" si="15"/>
-        <v>636615</v>
-      </c>
-      <c r="AE8">
-        <f t="shared" si="16"/>
-        <v>1.2824087637822457</v>
+        <v>1.0303285145229875</v>
       </c>
       <c r="AF8">
-        <v>579784</v>
+        <v>485745</v>
       </c>
       <c r="AG8">
-        <v>1174930</v>
+        <v>1052739</v>
       </c>
       <c r="AH8">
         <v>734915</v>
       </c>
       <c r="AI8">
+        <f t="shared" si="16"/>
+        <v>100109824</v>
+      </c>
+      <c r="AJ8">
         <f t="shared" si="17"/>
-        <v>115938880</v>
-      </c>
-      <c r="AJ8">
+        <v>31087680</v>
+      </c>
+      <c r="AK8">
         <f t="shared" si="18"/>
-        <v>37106176</v>
-      </c>
-      <c r="AK8">
-        <f t="shared" si="19"/>
-        <v>3.0829672732804685</v>
+        <v>2.6428662365158884</v>
       </c>
     </row>
     <row r="9" spans="1:37">
@@ -7548,126 +7557,125 @@
         <v>7</v>
       </c>
       <c r="D9">
-        <v>48148234</v>
+        <v>48969562</v>
       </c>
       <c r="E9">
+        <v>672566</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="0"/>
-        <v>1493894</v>
-      </c>
-      <c r="F9">
+        <v>1.3548291080511294</v>
+      </c>
+      <c r="G9">
+        <v>292544</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="1"/>
-        <v>3.0093270780011685</v>
-      </c>
-      <c r="G9">
-        <v>603538</v>
-      </c>
-      <c r="H9">
+        <v>86088448</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="2"/>
-        <v>95609216</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="3"/>
-        <v>38626432</v>
+        <v>37445632</v>
       </c>
       <c r="J9">
+        <f>(H9+I9)/S9</f>
+        <v>2.4884928381797011</v>
+      </c>
+      <c r="K9">
+        <v>49101958</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="4"/>
-        <v>2.7040671584425229</v>
-      </c>
-      <c r="K9">
-        <v>48982559</v>
-      </c>
-      <c r="L9">
+        <v>540170</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="5"/>
-        <v>659569</v>
-      </c>
-      <c r="M9">
+        <v>1.0881282123925065</v>
+      </c>
+      <c r="N9">
+        <v>301780</v>
+      </c>
+      <c r="O9">
+        <v>363688</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="6"/>
-        <v>1.3286477163106305</v>
-      </c>
-      <c r="N9">
-        <v>363909</v>
-      </c>
-      <c r="O9">
-        <v>412196</v>
-      </c>
-      <c r="P9">
+        <v>115693824</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="7"/>
-        <v>68592960</v>
-      </c>
-      <c r="Q9">
+        <v>38627840</v>
+      </c>
+      <c r="R9">
         <f t="shared" si="8"/>
-        <v>23290176</v>
-      </c>
-      <c r="R9">
-        <f t="shared" si="9"/>
-        <v>1.8509105008552413</v>
+        <v>3.1086834955987381</v>
       </c>
       <c r="S9">
         <v>49642128</v>
       </c>
       <c r="T9">
-        <v>49007722</v>
+        <v>49154511</v>
       </c>
       <c r="U9">
+        <f t="shared" si="9"/>
+        <v>487617</v>
+      </c>
+      <c r="V9">
         <f t="shared" si="10"/>
-        <v>634406</v>
-      </c>
-      <c r="V9">
+        <v>0.98226449921727765</v>
+      </c>
+      <c r="W9">
+        <v>316673</v>
+      </c>
+      <c r="X9">
+        <v>669522</v>
+      </c>
+      <c r="Y9">
         <f t="shared" si="11"/>
-        <v>1.2779589142512182</v>
-      </c>
-      <c r="W9">
-        <v>389990</v>
-      </c>
-      <c r="X9">
-        <v>738845</v>
-      </c>
-      <c r="Y9">
+        <v>148113792</v>
+      </c>
+      <c r="Z9">
         <f t="shared" si="12"/>
-        <v>87888064</v>
-      </c>
-      <c r="Z9">
+        <v>40534144</v>
+      </c>
+      <c r="AA9">
         <f t="shared" si="13"/>
-        <v>24959360</v>
-      </c>
-      <c r="AA9">
-        <f t="shared" si="14"/>
-        <v>2.2732189079404495</v>
+        <v>3.8001581237613342</v>
       </c>
       <c r="AB9">
         <v>49642128</v>
       </c>
       <c r="AC9">
-        <v>49000742</v>
+        <v>49175987</v>
       </c>
       <c r="AD9">
+        <f t="shared" si="14"/>
+        <v>466141</v>
+      </c>
+      <c r="AE9">
         <f t="shared" si="15"/>
-        <v>641386</v>
-      </c>
-      <c r="AE9">
-        <f t="shared" si="16"/>
-        <v>1.2920195524253111</v>
+        <v>0.93900285660598581</v>
       </c>
       <c r="AF9">
-        <v>411128</v>
+        <v>326988</v>
       </c>
       <c r="AG9">
-        <v>1123432</v>
+        <v>961065</v>
       </c>
       <c r="AH9">
         <v>800726</v>
       </c>
       <c r="AI9">
+        <f t="shared" si="16"/>
+        <v>182682368</v>
+      </c>
+      <c r="AJ9">
         <f t="shared" si="17"/>
-        <v>112948352</v>
-      </c>
-      <c r="AJ9">
+        <v>41854464</v>
+      </c>
+      <c r="AK9">
         <f t="shared" si="18"/>
-        <v>26312192</v>
-      </c>
-      <c r="AK9">
-        <f t="shared" si="19"/>
-        <v>2.805289571792732</v>
+        <v>4.5231105322479328</v>
       </c>
     </row>
     <row r="10" spans="1:37">
@@ -7681,126 +7689,125 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <v>48166766</v>
+        <v>49071087</v>
       </c>
       <c r="E10">
+        <v>571041</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="0"/>
-        <v>1475362</v>
-      </c>
-      <c r="F10">
+        <v>1.1503153128326811</v>
+      </c>
+      <c r="G10">
+        <v>221558</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="1"/>
-        <v>2.9719958822071448</v>
-      </c>
-      <c r="G10">
-        <v>522546</v>
-      </c>
-      <c r="H10">
+        <v>146186496</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="2"/>
-        <v>94423168</v>
-      </c>
-      <c r="I10">
+        <v>56718848</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="3"/>
-        <v>33442944</v>
-      </c>
-      <c r="J10">
+        <v>4.0873619277561994</v>
+      </c>
+      <c r="K10">
+        <v>49115716</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="4"/>
-        <v>2.5757580738682275</v>
-      </c>
-      <c r="K10">
-        <v>48938165</v>
-      </c>
-      <c r="L10">
+        <v>526412</v>
+      </c>
+      <c r="M10">
         <f t="shared" si="5"/>
-        <v>703963</v>
-      </c>
-      <c r="M10">
+        <v>1.0604138484957777</v>
+      </c>
+      <c r="N10">
+        <v>239893</v>
+      </c>
+      <c r="O10">
+        <v>365081</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="6"/>
-        <v>1.4180757923995524</v>
-      </c>
-      <c r="N10">
-        <v>314018</v>
-      </c>
-      <c r="O10">
-        <v>401439</v>
-      </c>
-      <c r="P10">
+        <v>228222208</v>
+      </c>
+      <c r="Q10">
         <f t="shared" si="7"/>
-        <v>70745728</v>
-      </c>
-      <c r="Q10">
+        <v>61412608</v>
+      </c>
+      <c r="R10">
         <f t="shared" si="8"/>
-        <v>20097152</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="9"/>
-        <v>1.8299553959491826</v>
+        <v>5.8344560893924609</v>
       </c>
       <c r="S10">
         <v>49642128</v>
       </c>
       <c r="T10">
-        <v>48922430</v>
+        <v>49129052</v>
       </c>
       <c r="U10">
+        <f t="shared" si="9"/>
+        <v>513076</v>
+      </c>
+      <c r="V10">
         <f t="shared" si="10"/>
-        <v>719698</v>
-      </c>
-      <c r="V10">
+        <v>1.0335495690273391</v>
+      </c>
+      <c r="W10">
+        <v>255620</v>
+      </c>
+      <c r="X10">
+        <v>737593</v>
+      </c>
+      <c r="Y10">
         <f t="shared" si="11"/>
-        <v>1.4497726608335566</v>
-      </c>
-      <c r="W10">
-        <v>343518</v>
-      </c>
-      <c r="X10">
-        <v>838762</v>
-      </c>
-      <c r="Y10">
+        <v>320171264</v>
+      </c>
+      <c r="Z10">
         <f t="shared" si="12"/>
-        <v>99741440</v>
-      </c>
-      <c r="Z10">
+        <v>65438720</v>
+      </c>
+      <c r="AA10">
         <f t="shared" si="13"/>
-        <v>21985152</v>
-      </c>
-      <c r="AA10">
-        <f t="shared" si="14"/>
-        <v>2.4520824731768145</v>
+        <v>7.7677972225525869</v>
       </c>
       <c r="AB10">
         <v>49642128</v>
       </c>
       <c r="AC10">
-        <v>48882542</v>
+        <v>49128105</v>
       </c>
       <c r="AD10">
+        <f t="shared" si="14"/>
+        <v>514023</v>
+      </c>
+      <c r="AE10">
         <f t="shared" si="15"/>
-        <v>759586</v>
-      </c>
-      <c r="AE10">
-        <f t="shared" si="16"/>
-        <v>1.5301237690696901</v>
+        <v>1.0354572229458012</v>
       </c>
       <c r="AF10">
-        <v>375098</v>
+        <v>271406</v>
       </c>
       <c r="AG10">
-        <v>1372112</v>
+        <v>1123099</v>
       </c>
       <c r="AH10">
         <v>906646</v>
       </c>
       <c r="AI10">
+        <f t="shared" si="16"/>
+        <v>419103232</v>
+      </c>
+      <c r="AJ10">
         <f t="shared" si="17"/>
-        <v>136428672</v>
-      </c>
-      <c r="AJ10">
+        <v>69479936</v>
+      </c>
+      <c r="AK10">
         <f t="shared" si="18"/>
-        <v>24006272</v>
-      </c>
-      <c r="AK10">
-        <f t="shared" si="19"/>
-        <v>3.231830512986873</v>
+        <v>9.8421076550143063</v>
       </c>
     </row>
     <row r="11" spans="1:37">
@@ -7814,126 +7821,125 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>47596171</v>
+        <v>48972332</v>
       </c>
       <c r="E11">
+        <v>669796</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="0"/>
-        <v>2045957</v>
-      </c>
-      <c r="F11">
+        <v>1.3492491699791758</v>
+      </c>
+      <c r="G11">
+        <v>247292</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="1"/>
-        <v>4.1214127645776992</v>
-      </c>
-      <c r="G11">
-        <v>683856</v>
-      </c>
-      <c r="H11">
+        <v>342935552</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="2"/>
-        <v>130941248</v>
-      </c>
-      <c r="I11">
+        <v>126613504</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="3"/>
-        <v>43766784</v>
-      </c>
-      <c r="J11">
+        <v>9.4586810621817019</v>
+      </c>
+      <c r="K11">
+        <v>48965714</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="4"/>
-        <v>3.5193501777361358</v>
-      </c>
-      <c r="K11">
-        <v>48660373</v>
-      </c>
-      <c r="L11">
+        <v>676414</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="5"/>
-        <v>981755</v>
-      </c>
-      <c r="M11">
+        <v>1.3625805888095692</v>
+      </c>
+      <c r="N11">
+        <v>282635</v>
+      </c>
+      <c r="O11">
+        <v>508242</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="6"/>
-        <v>1.9776650187115268</v>
-      </c>
-      <c r="N11">
-        <v>392997</v>
-      </c>
-      <c r="O11">
-        <v>548127</v>
-      </c>
-      <c r="P11">
+        <v>606543872</v>
+      </c>
+      <c r="Q11">
         <f t="shared" si="7"/>
-        <v>97912448</v>
-      </c>
-      <c r="Q11">
+        <v>144709120</v>
+      </c>
+      <c r="R11">
         <f t="shared" si="8"/>
-        <v>25151808</v>
-      </c>
-      <c r="R11">
-        <f t="shared" si="9"/>
-        <v>2.479028618595883</v>
+        <v>15.133376071227245</v>
       </c>
       <c r="S11">
         <v>49642128</v>
       </c>
       <c r="T11">
-        <v>48634651</v>
+        <v>48938867</v>
       </c>
       <c r="U11">
+        <f t="shared" si="9"/>
+        <v>703261</v>
+      </c>
+      <c r="V11">
         <f t="shared" si="10"/>
-        <v>1007477</v>
-      </c>
-      <c r="V11">
+        <v>1.4166616709098367</v>
+      </c>
+      <c r="W11">
+        <v>311568</v>
+      </c>
+      <c r="X11">
+        <v>1096234</v>
+      </c>
+      <c r="Y11">
         <f t="shared" si="11"/>
-        <v>2.0294798804757122</v>
-      </c>
-      <c r="W11">
-        <v>411911</v>
-      </c>
-      <c r="X11">
-        <v>1241899</v>
-      </c>
-      <c r="Y11">
+        <v>921341440</v>
+      </c>
+      <c r="Z11">
         <f t="shared" si="12"/>
-        <v>143960064</v>
-      </c>
-      <c r="Z11">
+        <v>159522816</v>
+      </c>
+      <c r="AA11">
         <f t="shared" si="13"/>
-        <v>26362304</v>
-      </c>
-      <c r="AA11">
-        <f t="shared" si="14"/>
-        <v>3.4310045693448115</v>
+        <v>21.773124955481361</v>
       </c>
       <c r="AB11">
         <v>49642128</v>
       </c>
       <c r="AC11">
-        <v>48511929</v>
+        <v>48918851</v>
       </c>
       <c r="AD11">
+        <f t="shared" si="14"/>
+        <v>723277</v>
+      </c>
+      <c r="AE11">
         <f t="shared" si="15"/>
-        <v>1130199</v>
-      </c>
-      <c r="AE11">
-        <f t="shared" si="16"/>
-        <v>2.2766932956621035</v>
+        <v>1.4569822631294129</v>
       </c>
       <c r="AF11">
-        <v>463548</v>
+        <v>323265</v>
       </c>
       <c r="AG11">
-        <v>2157510</v>
+        <v>1709101</v>
       </c>
       <c r="AH11">
         <v>1233087</v>
       </c>
       <c r="AI11">
+        <f t="shared" si="16"/>
+        <v>1245377536</v>
+      </c>
+      <c r="AJ11">
         <f t="shared" si="17"/>
-        <v>210413376</v>
-      </c>
-      <c r="AJ11">
+        <v>165511680</v>
+      </c>
+      <c r="AK11">
         <f t="shared" si="18"/>
-        <v>29667072</v>
-      </c>
-      <c r="AK11">
-        <f t="shared" si="19"/>
-        <v>4.8362239426964129</v>
+        <v>28.421207406741306</v>
       </c>
     </row>
     <row r="12" spans="1:37">
@@ -7947,189 +7953,166 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>47030974</v>
+        <v>48679020</v>
       </c>
       <c r="E12">
+        <v>963108</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="0"/>
-        <v>2611154</v>
-      </c>
-      <c r="F12">
+        <v>1.9401021648387033</v>
+      </c>
+      <c r="G12">
+        <v>327111</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="1"/>
-        <v>5.2599558181712114</v>
-      </c>
-      <c r="G12">
-        <v>771229</v>
-      </c>
-      <c r="H12">
+        <v>986222592</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="2"/>
-        <v>167113856</v>
-      </c>
-      <c r="I12">
+        <v>334961664</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="3"/>
-        <v>49358656</v>
-      </c>
-      <c r="J12">
+        <v>26.614174476968433</v>
+      </c>
+      <c r="K12">
+        <v>48609595</v>
+      </c>
+      <c r="L12">
         <f t="shared" si="4"/>
-        <v>4.3606614124197094</v>
-      </c>
-      <c r="K12">
-        <v>48285672</v>
-      </c>
-      <c r="L12">
+        <v>1032533</v>
+      </c>
+      <c r="M12">
         <f t="shared" si="5"/>
-        <v>1356456</v>
-      </c>
-      <c r="M12">
+        <v>2.0799531398009368</v>
+      </c>
+      <c r="N12">
+        <v>373596</v>
+      </c>
+      <c r="O12">
+        <v>814000</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="6"/>
-        <v>2.7324694864007442</v>
-      </c>
-      <c r="N12">
-        <v>427688</v>
-      </c>
-      <c r="O12">
-        <v>785875</v>
-      </c>
-      <c r="P12">
+        <v>1890849792</v>
+      </c>
+      <c r="Q12">
         <f t="shared" si="7"/>
-        <v>137109184</v>
-      </c>
-      <c r="Q12">
+        <v>382562304</v>
+      </c>
+      <c r="R12">
         <f t="shared" si="8"/>
-        <v>27372032</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="9"/>
-        <v>3.3133393475799426</v>
+        <v>45.796024215561431</v>
       </c>
       <c r="S12">
         <v>49642128</v>
       </c>
       <c r="T12">
-        <v>48121759</v>
+        <v>48553753</v>
       </c>
       <c r="U12">
+        <f t="shared" si="9"/>
+        <v>1088375</v>
+      </c>
+      <c r="V12">
         <f t="shared" si="10"/>
-        <v>1520369</v>
-      </c>
-      <c r="V12">
+        <v>2.1924422740298324</v>
+      </c>
+      <c r="W12">
+        <v>397816</v>
+      </c>
+      <c r="X12">
+        <v>1775001</v>
+      </c>
+      <c r="Y12">
         <f t="shared" si="11"/>
-        <v>3.0626587965769718</v>
-      </c>
-      <c r="W12">
-        <v>495311</v>
-      </c>
-      <c r="X12">
-        <v>1928568</v>
-      </c>
-      <c r="Y12">
+        <v>2932097024</v>
+      </c>
+      <c r="Z12">
         <f t="shared" si="12"/>
-        <v>220731968</v>
-      </c>
-      <c r="Z12">
+        <v>407363584</v>
+      </c>
+      <c r="AA12">
         <f t="shared" si="13"/>
-        <v>31699904</v>
-      </c>
-      <c r="AA12">
-        <f t="shared" si="14"/>
-        <v>5.0850332604597446</v>
+        <v>67.270698145736219</v>
       </c>
       <c r="AB12">
         <v>49642128</v>
       </c>
       <c r="AC12">
-        <v>47910528</v>
+        <v>48501934</v>
       </c>
       <c r="AD12">
+        <f t="shared" si="14"/>
+        <v>1140194</v>
+      </c>
+      <c r="AE12">
         <f t="shared" si="15"/>
-        <v>1731600</v>
-      </c>
-      <c r="AE12">
-        <f t="shared" si="16"/>
-        <v>3.488166341297859</v>
+        <v>2.2968274043368972</v>
       </c>
       <c r="AF12">
-        <v>574577</v>
+        <v>415177</v>
       </c>
       <c r="AG12">
-        <v>3488861</v>
+        <v>2876812</v>
       </c>
       <c r="AH12">
         <v>1705939</v>
       </c>
       <c r="AI12">
+        <f t="shared" si="16"/>
+        <v>4113414144</v>
+      </c>
+      <c r="AJ12">
         <f t="shared" si="17"/>
-        <v>334109504</v>
-      </c>
-      <c r="AJ12">
+        <v>425141248</v>
+      </c>
+      <c r="AK12">
         <f t="shared" si="18"/>
-        <v>36772928</v>
-      </c>
-      <c r="AK12">
-        <f t="shared" si="19"/>
-        <v>7.4711227528360586</v>
+        <v>91.425480229211772</v>
       </c>
     </row>
     <row r="13" spans="1:37">
       <c r="J13">
         <f>J4+J5+J6+J7+J8+J9+J10+J11+J12</f>
-        <v>87.603913192440075</v>
+        <v>50.058783378504643</v>
       </c>
       <c r="AK13">
         <f>AK4+AK5+AK7+AK6+AK8+AK9+AK10+AK11+AK12</f>
-        <v>67.535762044689136</v>
+        <v>142.92874753475516</v>
       </c>
     </row>
-    <row r="18" spans="44:46">
-      <c r="AR18" s="27"/>
-      <c r="AS18" s="28"/>
-      <c r="AT18" s="28"/>
+    <row r="65" spans="2:2">
+      <c r="B65" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="19" spans="44:46">
-      <c r="AR19" s="19"/>
-      <c r="AS19" s="21"/>
-      <c r="AT19" s="21"/>
+    <row r="66" spans="2:2">
+      <c r="B66" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="20" spans="44:46">
-      <c r="AR20" t="s">
-        <v>82</v>
-      </c>
-      <c r="AS20" t="s">
-        <v>83</v>
-      </c>
-      <c r="AT20" t="s">
-        <v>84</v>
+    <row r="67" spans="2:2">
+      <c r="B67" t="s">
+        <v>92</v>
       </c>
     </row>
-    <row r="75" spans="2:2">
-      <c r="B75" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2">
-      <c r="B76" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2">
-      <c r="B77" t="s">
+    <row r="68" spans="2:2">
+      <c r="B68" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2">
-      <c r="B78" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="AR18:AT18"/>
+  <mergeCells count="7">
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="P2:R2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="T1:AA1"/>
-    <mergeCell ref="AC1:AF1"/>
-    <mergeCell ref="AI1:AK1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>